<commit_message>
updated lab02 due date
</commit_message>
<xml_diff>
--- a/CS320-Spring2019Calendar.xlsx
+++ b/CS320-Spring2019Calendar.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="74">
   <si>
     <t>Monday</t>
   </si>
@@ -318,11 +318,6 @@
 (Marmoset)</t>
   </si>
   <si>
-    <t>Lab 2: Web Apps I due
-7:00 am
-(Marmoset)</t>
-  </si>
-  <si>
     <t>A01: Team Project Proposal due
 7:00 am
 (Google Doc)</t>
@@ -385,6 +380,18 @@
     <t>A06: Team Problem Domain Analysis due
 7:00 am
 (Violet UML &amp; Google Doc)</t>
+  </si>
+  <si>
+    <t>Lab 2: Web Apps I due
+for 110%
+7:00 am
+(Marmoset)</t>
+  </si>
+  <si>
+    <t>Lab 2: Web Apps I due
+for 100%
+7:00 am
+(Marmoset)</t>
   </si>
 </sst>
 </file>
@@ -1363,32 +1370,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1396,6 +1382,42 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1404,21 +1426,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1726,8 +1733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,17 +1752,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="120" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="121"/>
-      <c r="H1" s="121"/>
-      <c r="I1" s="122"/>
+      <c r="A1" s="131" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
+      <c r="H1" s="132"/>
+      <c r="I1" s="133"/>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1785,10 +1792,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="126">
+      <c r="A3" s="127">
         <v>16</v>
       </c>
-      <c r="B3" s="129" t="s">
+      <c r="B3" s="122" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="55">
@@ -1821,7 +1828,7 @@
     </row>
     <row r="4" spans="1:13" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="125"/>
-      <c r="B4" s="130"/>
+      <c r="B4" s="123"/>
       <c r="C4" s="53" t="s">
         <v>8</v>
       </c>
@@ -1844,7 +1851,7 @@
       <c r="A5" s="125">
         <v>15</v>
       </c>
-      <c r="B5" s="130"/>
+      <c r="B5" s="123"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>27</v>
@@ -1874,8 +1881,8 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="127"/>
-      <c r="B6" s="130"/>
+      <c r="A6" s="128"/>
+      <c r="B6" s="123"/>
       <c r="C6" s="88" t="s">
         <v>58</v>
       </c>
@@ -1887,18 +1894,20 @@
         <v>44</v>
       </c>
       <c r="G6" s="83" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="H6" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="78"/>
+      <c r="I6" s="51" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="126">
+      <c r="A7" s="127">
         <v>14</v>
       </c>
-      <c r="B7" s="131" t="s">
+      <c r="B7" s="136" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="91">
@@ -1931,10 +1940,10 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="128"/>
-      <c r="B8" s="132"/>
+      <c r="A8" s="126"/>
+      <c r="B8" s="137"/>
       <c r="C8" s="52" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="79" t="s">
         <v>35</v>
@@ -1948,14 +1957,14 @@
         <v>48</v>
       </c>
       <c r="I8" s="51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="124">
+      <c r="A9" s="135">
         <v>13</v>
       </c>
-      <c r="B9" s="132"/>
+      <c r="B9" s="137"/>
       <c r="C9" s="18">
         <f>I7 + 1</f>
         <v>10</v>
@@ -1987,9 +1996,9 @@
     </row>
     <row r="10" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="125"/>
-      <c r="B10" s="132"/>
+      <c r="B10" s="137"/>
       <c r="C10" s="52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>47</v>
@@ -2008,7 +2017,7 @@
       <c r="A11" s="125">
         <v>12</v>
       </c>
-      <c r="B11" s="132"/>
+      <c r="B11" s="137"/>
       <c r="C11" s="21">
         <f>I9 + 1</f>
         <v>17</v>
@@ -2040,9 +2049,9 @@
     </row>
     <row r="12" spans="1:13" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="125"/>
-      <c r="B12" s="132"/>
+      <c r="B12" s="137"/>
       <c r="C12" s="52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>49</v>
@@ -2061,7 +2070,7 @@
       <c r="A13" s="125">
         <v>11</v>
       </c>
-      <c r="B13" s="132"/>
+      <c r="B13" s="137"/>
       <c r="C13" s="21">
         <f>I11 + 1</f>
         <v>24</v>
@@ -2091,8 +2100,8 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="128"/>
-      <c r="B14" s="132"/>
+      <c r="A14" s="126"/>
+      <c r="B14" s="137"/>
       <c r="C14" s="96"/>
       <c r="D14" s="44" t="s">
         <v>19</v>
@@ -2102,7 +2111,7 @@
         <v>20</v>
       </c>
       <c r="G14" s="51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H14" s="10" t="s">
         <v>21</v>
@@ -2114,10 +2123,10 @@
       <c r="M14" s="38"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="126">
+      <c r="A15" s="127">
         <v>10</v>
       </c>
-      <c r="B15" s="131" t="s">
+      <c r="B15" s="136" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="55">
@@ -2150,8 +2159,8 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="127"/>
-      <c r="B16" s="133"/>
+      <c r="A16" s="128"/>
+      <c r="B16" s="138"/>
       <c r="C16" s="60" t="s">
         <v>30</v>
       </c>
@@ -2287,19 +2296,19 @@
       <c r="I25" s="30"/>
     </row>
     <row r="26" spans="1:11" s="32" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="120" t="str">
+      <c r="A26" s="131" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2019 Schedule
 (as of 1-30-2019, subject to change)</v>
       </c>
-      <c r="B26" s="121"/>
-      <c r="C26" s="121"/>
-      <c r="D26" s="121"/>
-      <c r="E26" s="121"/>
-      <c r="F26" s="121"/>
-      <c r="G26" s="121"/>
-      <c r="H26" s="121"/>
-      <c r="I26" s="122"/>
+      <c r="B26" s="132"/>
+      <c r="C26" s="132"/>
+      <c r="D26" s="132"/>
+      <c r="E26" s="132"/>
+      <c r="F26" s="132"/>
+      <c r="G26" s="132"/>
+      <c r="H26" s="132"/>
+      <c r="I26" s="133"/>
     </row>
     <row r="27" spans="1:11" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
@@ -2337,7 +2346,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="123">
+      <c r="A28" s="134">
         <v>10</v>
       </c>
       <c r="B28" s="80"/>
@@ -2371,8 +2380,8 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="124"/>
-      <c r="B29" s="130" t="s">
+      <c r="A29" s="135"/>
+      <c r="B29" s="123" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="101" t="s">
@@ -2404,10 +2413,10 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="124">
+      <c r="A30" s="135">
         <v>9</v>
       </c>
-      <c r="B30" s="130"/>
+      <c r="B30" s="123"/>
       <c r="C30" s="100">
         <f>I15 + 1</f>
         <v>10</v>
@@ -2439,7 +2448,7 @@
     </row>
     <row r="31" spans="1:11" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="125"/>
-      <c r="B31" s="130"/>
+      <c r="B31" s="123"/>
       <c r="C31" s="53" t="str">
         <f>I29</f>
         <v>WINTER BREAK</v>
@@ -2448,7 +2457,7 @@
         <v>26</v>
       </c>
       <c r="E31" s="50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>27</v>
@@ -2458,7 +2467,7 @@
         <v>28</v>
       </c>
       <c r="I31" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K31" s="39"/>
     </row>
@@ -2466,7 +2475,7 @@
       <c r="A32" s="125">
         <v>8</v>
       </c>
-      <c r="B32" s="130"/>
+      <c r="B32" s="123"/>
       <c r="C32" s="25">
         <f>I30 + 1</f>
         <v>17</v>
@@ -2498,7 +2507,7 @@
     </row>
     <row r="33" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="125"/>
-      <c r="B33" s="130"/>
+      <c r="B33" s="123"/>
       <c r="C33" s="10"/>
       <c r="D33" s="40" t="s">
         <v>42</v>
@@ -2512,7 +2521,7 @@
         <v>22</v>
       </c>
       <c r="I33" s="51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K33" s="37"/>
     </row>
@@ -2520,7 +2529,7 @@
       <c r="A34" s="125">
         <v>7</v>
       </c>
-      <c r="B34" s="130"/>
+      <c r="B34" s="123"/>
       <c r="C34" s="10">
         <f>I32 + 1</f>
         <v>24</v>
@@ -2552,7 +2561,7 @@
     </row>
     <row r="35" spans="1:11" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="125"/>
-      <c r="B35" s="130"/>
+      <c r="B35" s="123"/>
       <c r="C35" s="10"/>
       <c r="D35" s="102" t="s">
         <v>16</v>
@@ -2601,7 +2610,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="127"/>
+      <c r="A37" s="128"/>
       <c r="B37" s="82"/>
       <c r="C37" s="116"/>
       <c r="D37" s="115" t="s">
@@ -2618,10 +2627,10 @@
       <c r="I37" s="46"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="126">
+      <c r="A38" s="127">
         <v>5</v>
       </c>
-      <c r="B38" s="134" t="s">
+      <c r="B38" s="120" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="48">
@@ -2655,13 +2664,13 @@
     </row>
     <row r="39" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="125"/>
-      <c r="B39" s="135"/>
+      <c r="B39" s="121"/>
       <c r="C39" s="48"/>
       <c r="D39" s="28" t="s">
         <v>39</v>
       </c>
       <c r="E39" s="117" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F39" s="27" t="s">
         <v>55</v>
@@ -2676,7 +2685,7 @@
       <c r="A40" s="125">
         <v>4</v>
       </c>
-      <c r="B40" s="135"/>
+      <c r="B40" s="121"/>
       <c r="C40" s="21">
         <f>I38 + 1</f>
         <v>14</v>
@@ -2708,13 +2717,13 @@
     </row>
     <row r="41" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="125"/>
-      <c r="B41" s="135"/>
+      <c r="B41" s="121"/>
       <c r="C41" s="47"/>
       <c r="D41" s="108" t="s">
         <v>54</v>
       </c>
       <c r="E41" s="106" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F41" s="112" t="s">
         <v>55</v>
@@ -2733,7 +2742,7 @@
       <c r="A42" s="125">
         <v>3</v>
       </c>
-      <c r="B42" s="135"/>
+      <c r="B42" s="121"/>
       <c r="C42" s="53">
         <f>I40 + 1</f>
         <v>21</v>
@@ -2765,7 +2774,7 @@
     </row>
     <row r="43" spans="1:11" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="125"/>
-      <c r="B43" s="135"/>
+      <c r="B43" s="121"/>
       <c r="C43" s="53" t="s">
         <v>6</v>
       </c>
@@ -2786,7 +2795,7 @@
       <c r="A44" s="125">
         <v>2</v>
       </c>
-      <c r="B44" s="135"/>
+      <c r="B44" s="121"/>
       <c r="C44" s="21">
         <f>I42 + 1</f>
         <v>28</v>
@@ -2816,8 +2825,8 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="127"/>
-      <c r="B45" s="135"/>
+      <c r="A45" s="128"/>
+      <c r="B45" s="121"/>
       <c r="C45" s="107"/>
       <c r="D45" s="102" t="s">
         <v>41</v>
@@ -2833,11 +2842,11 @@
       <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="126">
+      <c r="A46" s="127">
         <f>A49 + 1</f>
         <v>1</v>
       </c>
-      <c r="B46" s="129" t="s">
+      <c r="B46" s="122" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="41">
@@ -2871,7 +2880,7 @@
     </row>
     <row r="47" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="125"/>
-      <c r="B47" s="130"/>
+      <c r="B47" s="123"/>
       <c r="C47" s="42"/>
       <c r="D47" s="7" t="s">
         <v>7</v>
@@ -2883,14 +2892,14 @@
       <c r="G47" s="49"/>
       <c r="H47" s="8"/>
       <c r="I47" s="51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="137">
+      <c r="A48" s="129">
         <v>0</v>
       </c>
-      <c r="B48" s="130"/>
+      <c r="B48" s="123"/>
       <c r="C48" s="25">
         <f>I46 + 1</f>
         <v>12</v>
@@ -2921,14 +2930,14 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="138.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="138"/>
-      <c r="B49" s="136"/>
+      <c r="A49" s="130"/>
+      <c r="B49" s="124"/>
       <c r="C49" s="12"/>
       <c r="D49" s="29" t="s">
         <v>57</v>
       </c>
       <c r="E49" s="75" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F49" s="29" t="s">
         <v>56</v>
@@ -2940,6 +2949,19 @@
     <row r="50" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B14"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B29:B35"/>
     <mergeCell ref="B38:B45"/>
     <mergeCell ref="B46:B49"/>
     <mergeCell ref="A13:A14"/>
@@ -2953,19 +2975,6 @@
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B14"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B29:B35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated due date for assign05
</commit_message>
<xml_diff>
--- a/CS320-Spring2019Calendar.xlsx
+++ b/CS320-Spring2019Calendar.xlsx
@@ -273,11 +273,6 @@
   </si>
   <si>
     <t>Team Session:
-Textual Analysis
-(in class)</t>
-  </si>
-  <si>
-    <t>Team Session:
 Analysis Model (UML)
 (in class)</t>
   </si>
@@ -333,12 +328,6 @@
 (Marmoset)</t>
   </si>
   <si>
-    <t>A05: Team
-Use Cases due
-7:00 am
-(Google Doc)</t>
-  </si>
-  <si>
     <t>Lab 4: SQL due
 7:00 am
 (Marmoset)</t>
@@ -373,10 +362,6 @@
 both 7:00 am (Marmoset)</t>
   </si>
   <si>
-    <t>CS320: SW Engineering - Spring 2019 Schedule
-(as of 1-30-2019, subject to change)</t>
-  </si>
-  <si>
     <t>A06: Team Problem Domain Analysis due
 7:00 am
 (Violet UML &amp; Google Doc)</t>
@@ -392,6 +377,36 @@
 for 100%
 7:00 am
 (Marmoset)</t>
+  </si>
+  <si>
+    <t>CS320: SW Engineering - Spring 2019 Schedule
+(as of 2-15-2019, subject to change)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Team Session:
+Textual Analysis
+(in class)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A05: Use Cases due, 7:00 am</t>
+    </r>
+  </si>
+  <si>
+    <t>A05: Team
+Use Cases due
+7:00 am
+MON, 2-18 --&gt;
+(Google Doc)</t>
   </si>
 </sst>
 </file>
@@ -1011,7 +1026,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1370,62 +1385,65 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1733,8 +1751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,17 +1770,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="131" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="133"/>
+      <c r="A1" s="120" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="122"/>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1792,10 +1810,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="127">
+      <c r="A3" s="126">
         <v>16</v>
       </c>
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="129" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="55">
@@ -1828,7 +1846,7 @@
     </row>
     <row r="4" spans="1:13" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="125"/>
-      <c r="B4" s="123"/>
+      <c r="B4" s="130"/>
       <c r="C4" s="53" t="s">
         <v>8</v>
       </c>
@@ -1851,7 +1869,7 @@
       <c r="A5" s="125">
         <v>15</v>
       </c>
-      <c r="B5" s="123"/>
+      <c r="B5" s="130"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>27</v>
@@ -1881,10 +1899,10 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="128"/>
-      <c r="B6" s="123"/>
+      <c r="A6" s="127"/>
+      <c r="B6" s="130"/>
       <c r="C6" s="88" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="89" t="s">
         <v>43</v>
@@ -1894,20 +1912,20 @@
         <v>44</v>
       </c>
       <c r="G6" s="83" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H6" s="119" t="s">
         <v>45</v>
       </c>
       <c r="I6" s="51" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="127">
+      <c r="A7" s="126">
         <v>14</v>
       </c>
-      <c r="B7" s="136" t="s">
+      <c r="B7" s="131" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="91">
@@ -1940,10 +1958,10 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="126"/>
-      <c r="B8" s="137"/>
+      <c r="A8" s="128"/>
+      <c r="B8" s="132"/>
       <c r="C8" s="52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="79" t="s">
         <v>35</v>
@@ -1957,14 +1975,14 @@
         <v>48</v>
       </c>
       <c r="I8" s="51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="135">
+      <c r="A9" s="124">
         <v>13</v>
       </c>
-      <c r="B9" s="137"/>
+      <c r="B9" s="132"/>
       <c r="C9" s="18">
         <f>I7 + 1</f>
         <v>10</v>
@@ -1996,16 +2014,16 @@
     </row>
     <row r="10" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="125"/>
-      <c r="B10" s="137"/>
+      <c r="B10" s="132"/>
       <c r="C10" s="52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>47</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="16" t="s">
@@ -2017,7 +2035,7 @@
       <c r="A11" s="125">
         <v>12</v>
       </c>
-      <c r="B11" s="137"/>
+      <c r="B11" s="132"/>
       <c r="C11" s="21">
         <f>I9 + 1</f>
         <v>17</v>
@@ -2049,20 +2067,20 @@
     </row>
     <row r="12" spans="1:13" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="125"/>
-      <c r="B12" s="137"/>
+      <c r="B12" s="132"/>
       <c r="C12" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>49</v>
+        <v>73</v>
+      </c>
+      <c r="D12" s="139" t="s">
+        <v>72</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I12" s="94"/>
     </row>
@@ -2070,7 +2088,7 @@
       <c r="A13" s="125">
         <v>11</v>
       </c>
-      <c r="B13" s="137"/>
+      <c r="B13" s="132"/>
       <c r="C13" s="21">
         <f>I11 + 1</f>
         <v>24</v>
@@ -2100,8 +2118,8 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="126"/>
-      <c r="B14" s="137"/>
+      <c r="A14" s="128"/>
+      <c r="B14" s="132"/>
       <c r="C14" s="96"/>
       <c r="D14" s="44" t="s">
         <v>19</v>
@@ -2111,7 +2129,7 @@
         <v>20</v>
       </c>
       <c r="G14" s="51" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H14" s="10" t="s">
         <v>21</v>
@@ -2123,10 +2141,10 @@
       <c r="M14" s="38"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="127">
+      <c r="A15" s="126">
         <v>10</v>
       </c>
-      <c r="B15" s="136" t="s">
+      <c r="B15" s="131" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="55">
@@ -2159,8 +2177,8 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="128"/>
-      <c r="B16" s="138"/>
+      <c r="A16" s="127"/>
+      <c r="B16" s="133"/>
       <c r="C16" s="60" t="s">
         <v>30</v>
       </c>
@@ -2296,19 +2314,19 @@
       <c r="I25" s="30"/>
     </row>
     <row r="26" spans="1:11" s="32" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="131" t="str">
+      <c r="A26" s="120" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2019 Schedule
-(as of 1-30-2019, subject to change)</v>
-      </c>
-      <c r="B26" s="132"/>
-      <c r="C26" s="132"/>
-      <c r="D26" s="132"/>
-      <c r="E26" s="132"/>
-      <c r="F26" s="132"/>
-      <c r="G26" s="132"/>
-      <c r="H26" s="132"/>
-      <c r="I26" s="133"/>
+(as of 2-15-2019, subject to change)</v>
+      </c>
+      <c r="B26" s="121"/>
+      <c r="C26" s="121"/>
+      <c r="D26" s="121"/>
+      <c r="E26" s="121"/>
+      <c r="F26" s="121"/>
+      <c r="G26" s="121"/>
+      <c r="H26" s="121"/>
+      <c r="I26" s="122"/>
     </row>
     <row r="27" spans="1:11" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
@@ -2346,7 +2364,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="134">
+      <c r="A28" s="123">
         <v>10</v>
       </c>
       <c r="B28" s="80"/>
@@ -2380,8 +2398,8 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="135"/>
-      <c r="B29" s="123" t="s">
+      <c r="A29" s="124"/>
+      <c r="B29" s="130" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="101" t="s">
@@ -2413,10 +2431,10 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="135">
+      <c r="A30" s="124">
         <v>9</v>
       </c>
-      <c r="B30" s="123"/>
+      <c r="B30" s="130"/>
       <c r="C30" s="100">
         <f>I15 + 1</f>
         <v>10</v>
@@ -2448,7 +2466,7 @@
     </row>
     <row r="31" spans="1:11" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="125"/>
-      <c r="B31" s="123"/>
+      <c r="B31" s="130"/>
       <c r="C31" s="53" t="str">
         <f>I29</f>
         <v>WINTER BREAK</v>
@@ -2457,7 +2475,7 @@
         <v>26</v>
       </c>
       <c r="E31" s="50" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>27</v>
@@ -2467,7 +2485,7 @@
         <v>28</v>
       </c>
       <c r="I31" s="51" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K31" s="39"/>
     </row>
@@ -2475,7 +2493,7 @@
       <c r="A32" s="125">
         <v>8</v>
       </c>
-      <c r="B32" s="123"/>
+      <c r="B32" s="130"/>
       <c r="C32" s="25">
         <f>I30 + 1</f>
         <v>17</v>
@@ -2507,7 +2525,7 @@
     </row>
     <row r="33" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="125"/>
-      <c r="B33" s="123"/>
+      <c r="B33" s="130"/>
       <c r="C33" s="10"/>
       <c r="D33" s="40" t="s">
         <v>42</v>
@@ -2521,7 +2539,7 @@
         <v>22</v>
       </c>
       <c r="I33" s="51" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K33" s="37"/>
     </row>
@@ -2529,7 +2547,7 @@
       <c r="A34" s="125">
         <v>7</v>
       </c>
-      <c r="B34" s="123"/>
+      <c r="B34" s="130"/>
       <c r="C34" s="10">
         <f>I32 + 1</f>
         <v>24</v>
@@ -2561,7 +2579,7 @@
     </row>
     <row r="35" spans="1:11" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="125"/>
-      <c r="B35" s="123"/>
+      <c r="B35" s="130"/>
       <c r="C35" s="10"/>
       <c r="D35" s="102" t="s">
         <v>16</v>
@@ -2572,7 +2590,7 @@
       </c>
       <c r="G35" s="90"/>
       <c r="H35" s="89" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I35" s="77"/>
     </row>
@@ -2610,11 +2628,11 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="128"/>
+      <c r="A37" s="127"/>
       <c r="B37" s="82"/>
       <c r="C37" s="116"/>
       <c r="D37" s="115" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E37" s="87"/>
       <c r="F37" s="79" t="s">
@@ -2627,10 +2645,10 @@
       <c r="I37" s="46"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="127">
+      <c r="A38" s="126">
         <v>5</v>
       </c>
-      <c r="B38" s="120" t="s">
+      <c r="B38" s="134" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="48">
@@ -2664,20 +2682,20 @@
     </row>
     <row r="39" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="125"/>
-      <c r="B39" s="121"/>
+      <c r="B39" s="135"/>
       <c r="C39" s="48"/>
       <c r="D39" s="28" t="s">
         <v>39</v>
       </c>
       <c r="E39" s="117" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F39" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G39" s="15"/>
       <c r="H39" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I39" s="78"/>
     </row>
@@ -2685,7 +2703,7 @@
       <c r="A40" s="125">
         <v>4</v>
       </c>
-      <c r="B40" s="121"/>
+      <c r="B40" s="135"/>
       <c r="C40" s="21">
         <f>I38 + 1</f>
         <v>14</v>
@@ -2717,16 +2735,16 @@
     </row>
     <row r="41" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="125"/>
-      <c r="B41" s="121"/>
+      <c r="B41" s="135"/>
       <c r="C41" s="47"/>
       <c r="D41" s="108" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" s="106" t="s">
+        <v>65</v>
+      </c>
+      <c r="F41" s="112" t="s">
         <v>54</v>
-      </c>
-      <c r="E41" s="106" t="s">
-        <v>67</v>
-      </c>
-      <c r="F41" s="112" t="s">
-        <v>55</v>
       </c>
       <c r="G41" s="57" t="s">
         <v>6</v>
@@ -2742,7 +2760,7 @@
       <c r="A42" s="125">
         <v>3</v>
       </c>
-      <c r="B42" s="121"/>
+      <c r="B42" s="135"/>
       <c r="C42" s="53">
         <f>I40 + 1</f>
         <v>21</v>
@@ -2774,7 +2792,7 @@
     </row>
     <row r="43" spans="1:11" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="125"/>
-      <c r="B43" s="121"/>
+      <c r="B43" s="135"/>
       <c r="C43" s="53" t="s">
         <v>6</v>
       </c>
@@ -2783,7 +2801,7 @@
       </c>
       <c r="E43" s="15"/>
       <c r="F43" s="105" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G43" s="97"/>
       <c r="H43" s="105" t="s">
@@ -2795,7 +2813,7 @@
       <c r="A44" s="125">
         <v>2</v>
       </c>
-      <c r="B44" s="121"/>
+      <c r="B44" s="135"/>
       <c r="C44" s="21">
         <f>I42 + 1</f>
         <v>28</v>
@@ -2825,8 +2843,8 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="128"/>
-      <c r="B45" s="121"/>
+      <c r="A45" s="127"/>
+      <c r="B45" s="135"/>
       <c r="C45" s="107"/>
       <c r="D45" s="102" t="s">
         <v>41</v>
@@ -2842,11 +2860,11 @@
       <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="127">
+      <c r="A46" s="126">
         <f>A49 + 1</f>
         <v>1</v>
       </c>
-      <c r="B46" s="122" t="s">
+      <c r="B46" s="129" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="41">
@@ -2880,7 +2898,7 @@
     </row>
     <row r="47" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="125"/>
-      <c r="B47" s="123"/>
+      <c r="B47" s="130"/>
       <c r="C47" s="42"/>
       <c r="D47" s="7" t="s">
         <v>7</v>
@@ -2892,14 +2910,14 @@
       <c r="G47" s="49"/>
       <c r="H47" s="8"/>
       <c r="I47" s="51" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="129">
+      <c r="A48" s="137">
         <v>0</v>
       </c>
-      <c r="B48" s="123"/>
+      <c r="B48" s="130"/>
       <c r="C48" s="25">
         <f>I46 + 1</f>
         <v>12</v>
@@ -2930,17 +2948,17 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="138.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="130"/>
-      <c r="B49" s="124"/>
+      <c r="A49" s="138"/>
+      <c r="B49" s="136"/>
       <c r="C49" s="12"/>
       <c r="D49" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E49" s="75" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F49" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G49" s="26"/>
       <c r="H49" s="12"/>
@@ -2949,6 +2967,19 @@
     <row r="50" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B38:B45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A31"/>
@@ -2962,19 +2993,6 @@
     <mergeCell ref="A26:I26"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B29:B35"/>
-    <mergeCell ref="B38:B45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated schedule due to snow day
</commit_message>
<xml_diff>
--- a/CS320-Spring2019Calendar.xlsx
+++ b/CS320-Spring2019Calendar.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
   <si>
     <t>Monday</t>
   </si>
@@ -277,10 +277,6 @@
 (in class)</t>
   </si>
   <si>
-    <t>Team Session: Analysis model presentation and discussion
-(in class)</t>
-  </si>
-  <si>
     <t>Team Session:
 Use Cases
 (in class)</t>
@@ -377,10 +373,6 @@
 for 100%
 7:00 am
 (Marmoset)</t>
-  </si>
-  <si>
-    <t>CS320: SW Engineering - Spring 2019 Schedule
-(as of 2-15-2019, subject to change)</t>
   </si>
   <si>
     <r>
@@ -407,6 +399,15 @@
 7:00 am
 MON, 2-18 --&gt;
 (Google Doc)</t>
+  </si>
+  <si>
+    <t>CS320: SW Engineering - Spring 2019 Schedule
+(as of 2-20-2019, subject to change)</t>
+  </si>
+  <si>
+    <t>WOO…! HOO…!
+A SNOW DAY
+(you're never too old to enjoy a snow day…  :-)</t>
   </si>
 </sst>
 </file>
@@ -1385,32 +1386,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1418,6 +1401,42 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1426,24 +1445,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1752,7 +1753,7 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1770,17 +1771,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="120" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="121"/>
-      <c r="H1" s="121"/>
-      <c r="I1" s="122"/>
+      <c r="A1" s="132" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="134"/>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1810,10 +1811,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="126">
+      <c r="A3" s="128">
         <v>16</v>
       </c>
-      <c r="B3" s="129" t="s">
+      <c r="B3" s="123" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="55">
@@ -1845,8 +1846,8 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="125"/>
-      <c r="B4" s="130"/>
+      <c r="A4" s="126"/>
+      <c r="B4" s="124"/>
       <c r="C4" s="53" t="s">
         <v>8</v>
       </c>
@@ -1866,10 +1867,10 @@
       <c r="I4" s="93"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="125">
+      <c r="A5" s="126">
         <v>15</v>
       </c>
-      <c r="B5" s="130"/>
+      <c r="B5" s="124"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>27</v>
@@ -1899,10 +1900,10 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="127"/>
-      <c r="B6" s="130"/>
+      <c r="A6" s="129"/>
+      <c r="B6" s="124"/>
       <c r="C6" s="88" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" s="89" t="s">
         <v>43</v>
@@ -1912,20 +1913,20 @@
         <v>44</v>
       </c>
       <c r="G6" s="83" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H6" s="119" t="s">
         <v>45</v>
       </c>
       <c r="I6" s="51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="126">
+      <c r="A7" s="128">
         <v>14</v>
       </c>
-      <c r="B7" s="131" t="s">
+      <c r="B7" s="137" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="91">
@@ -1958,10 +1959,10 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="128"/>
-      <c r="B8" s="132"/>
+      <c r="A8" s="127"/>
+      <c r="B8" s="138"/>
       <c r="C8" s="52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="79" t="s">
         <v>35</v>
@@ -1975,14 +1976,14 @@
         <v>48</v>
       </c>
       <c r="I8" s="51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="124">
+      <c r="A9" s="136">
         <v>13</v>
       </c>
-      <c r="B9" s="132"/>
+      <c r="B9" s="138"/>
       <c r="C9" s="18">
         <f>I7 + 1</f>
         <v>10</v>
@@ -2013,17 +2014,17 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="125"/>
-      <c r="B10" s="132"/>
+      <c r="A10" s="126"/>
+      <c r="B10" s="138"/>
       <c r="C10" s="52" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>47</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="16" t="s">
@@ -2032,10 +2033,10 @@
       <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="125">
+      <c r="A11" s="126">
         <v>12</v>
       </c>
-      <c r="B11" s="132"/>
+      <c r="B11" s="138"/>
       <c r="C11" s="21">
         <f>I9 + 1</f>
         <v>17</v>
@@ -2066,29 +2067,29 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="125"/>
-      <c r="B12" s="132"/>
+      <c r="A12" s="126"/>
+      <c r="B12" s="138"/>
       <c r="C12" s="52" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12" s="139" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="D12" s="120" t="s">
+        <v>70</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="16" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I12" s="94"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="125">
+      <c r="A13" s="126">
         <v>11</v>
       </c>
-      <c r="B13" s="132"/>
+      <c r="B13" s="138"/>
       <c r="C13" s="21">
         <f>I11 + 1</f>
         <v>24</v>
@@ -2118,8 +2119,8 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="128"/>
-      <c r="B14" s="132"/>
+      <c r="A14" s="127"/>
+      <c r="B14" s="138"/>
       <c r="C14" s="96"/>
       <c r="D14" s="44" t="s">
         <v>19</v>
@@ -2128,23 +2129,21 @@
       <c r="F14" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="51" t="s">
-        <v>68</v>
-      </c>
+      <c r="G14" s="78"/>
       <c r="H14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="58" t="s">
-        <v>30</v>
+      <c r="I14" s="51" t="s">
+        <v>67</v>
       </c>
       <c r="L14" s="38"/>
       <c r="M14" s="38"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="126">
+      <c r="A15" s="128">
         <v>10</v>
       </c>
-      <c r="B15" s="131" t="s">
+      <c r="B15" s="137" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="55">
@@ -2177,8 +2176,8 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="127"/>
-      <c r="B16" s="133"/>
+      <c r="A16" s="129"/>
+      <c r="B16" s="139"/>
       <c r="C16" s="60" t="s">
         <v>30</v>
       </c>
@@ -2314,19 +2313,19 @@
       <c r="I25" s="30"/>
     </row>
     <row r="26" spans="1:11" s="32" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="120" t="str">
+      <c r="A26" s="132" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2019 Schedule
-(as of 2-15-2019, subject to change)</v>
-      </c>
-      <c r="B26" s="121"/>
-      <c r="C26" s="121"/>
-      <c r="D26" s="121"/>
-      <c r="E26" s="121"/>
-      <c r="F26" s="121"/>
-      <c r="G26" s="121"/>
-      <c r="H26" s="121"/>
-      <c r="I26" s="122"/>
+(as of 2-20-2019, subject to change)</v>
+      </c>
+      <c r="B26" s="133"/>
+      <c r="C26" s="133"/>
+      <c r="D26" s="133"/>
+      <c r="E26" s="133"/>
+      <c r="F26" s="133"/>
+      <c r="G26" s="133"/>
+      <c r="H26" s="133"/>
+      <c r="I26" s="134"/>
     </row>
     <row r="27" spans="1:11" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
@@ -2364,7 +2363,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="123">
+      <c r="A28" s="135">
         <v>10</v>
       </c>
       <c r="B28" s="80"/>
@@ -2398,8 +2397,8 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="124"/>
-      <c r="B29" s="130" t="s">
+      <c r="A29" s="136"/>
+      <c r="B29" s="124" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="101" t="s">
@@ -2431,10 +2430,10 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="124">
+      <c r="A30" s="136">
         <v>9</v>
       </c>
-      <c r="B30" s="130"/>
+      <c r="B30" s="124"/>
       <c r="C30" s="100">
         <f>I15 + 1</f>
         <v>10</v>
@@ -2465,8 +2464,8 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="125"/>
-      <c r="B31" s="130"/>
+      <c r="A31" s="126"/>
+      <c r="B31" s="124"/>
       <c r="C31" s="53" t="str">
         <f>I29</f>
         <v>WINTER BREAK</v>
@@ -2475,7 +2474,7 @@
         <v>26</v>
       </c>
       <c r="E31" s="50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>27</v>
@@ -2485,15 +2484,15 @@
         <v>28</v>
       </c>
       <c r="I31" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K31" s="39"/>
     </row>
     <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="125">
+      <c r="A32" s="126">
         <v>8</v>
       </c>
-      <c r="B32" s="130"/>
+      <c r="B32" s="124"/>
       <c r="C32" s="25">
         <f>I30 + 1</f>
         <v>17</v>
@@ -2524,8 +2523,8 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="125"/>
-      <c r="B33" s="130"/>
+      <c r="A33" s="126"/>
+      <c r="B33" s="124"/>
       <c r="C33" s="10"/>
       <c r="D33" s="40" t="s">
         <v>42</v>
@@ -2539,15 +2538,15 @@
         <v>22</v>
       </c>
       <c r="I33" s="51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K33" s="37"/>
     </row>
     <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="125">
+      <c r="A34" s="126">
         <v>7</v>
       </c>
-      <c r="B34" s="130"/>
+      <c r="B34" s="124"/>
       <c r="C34" s="10">
         <f>I32 + 1</f>
         <v>24</v>
@@ -2578,8 +2577,8 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="125"/>
-      <c r="B35" s="130"/>
+      <c r="A35" s="126"/>
+      <c r="B35" s="124"/>
       <c r="C35" s="10"/>
       <c r="D35" s="102" t="s">
         <v>16</v>
@@ -2590,12 +2589,12 @@
       </c>
       <c r="G35" s="90"/>
       <c r="H35" s="89" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I35" s="77"/>
     </row>
     <row r="36" spans="1:11" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="125">
+      <c r="A36" s="126">
         <v>6</v>
       </c>
       <c r="B36" s="81"/>
@@ -2628,11 +2627,11 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="127"/>
+      <c r="A37" s="129"/>
       <c r="B37" s="82"/>
       <c r="C37" s="116"/>
       <c r="D37" s="115" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E37" s="87"/>
       <c r="F37" s="79" t="s">
@@ -2645,10 +2644,10 @@
       <c r="I37" s="46"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="126">
+      <c r="A38" s="128">
         <v>5</v>
       </c>
-      <c r="B38" s="134" t="s">
+      <c r="B38" s="121" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="48">
@@ -2681,29 +2680,29 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="125"/>
-      <c r="B39" s="135"/>
+      <c r="A39" s="126"/>
+      <c r="B39" s="122"/>
       <c r="C39" s="48"/>
       <c r="D39" s="28" t="s">
         <v>39</v>
       </c>
       <c r="E39" s="117" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F39" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G39" s="15"/>
       <c r="H39" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I39" s="78"/>
     </row>
     <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="125">
+      <c r="A40" s="126">
         <v>4</v>
       </c>
-      <c r="B40" s="135"/>
+      <c r="B40" s="122"/>
       <c r="C40" s="21">
         <f>I38 + 1</f>
         <v>14</v>
@@ -2734,17 +2733,17 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="125"/>
-      <c r="B41" s="135"/>
+      <c r="A41" s="126"/>
+      <c r="B41" s="122"/>
       <c r="C41" s="47"/>
       <c r="D41" s="108" t="s">
+        <v>52</v>
+      </c>
+      <c r="E41" s="106" t="s">
+        <v>64</v>
+      </c>
+      <c r="F41" s="112" t="s">
         <v>53</v>
-      </c>
-      <c r="E41" s="106" t="s">
-        <v>65</v>
-      </c>
-      <c r="F41" s="112" t="s">
-        <v>54</v>
       </c>
       <c r="G41" s="57" t="s">
         <v>6</v>
@@ -2757,10 +2756,10 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="125">
+      <c r="A42" s="126">
         <v>3</v>
       </c>
-      <c r="B42" s="135"/>
+      <c r="B42" s="122"/>
       <c r="C42" s="53">
         <f>I40 + 1</f>
         <v>21</v>
@@ -2791,8 +2790,8 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="125"/>
-      <c r="B43" s="135"/>
+      <c r="A43" s="126"/>
+      <c r="B43" s="122"/>
       <c r="C43" s="53" t="s">
         <v>6</v>
       </c>
@@ -2801,7 +2800,7 @@
       </c>
       <c r="E43" s="15"/>
       <c r="F43" s="105" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G43" s="97"/>
       <c r="H43" s="105" t="s">
@@ -2810,10 +2809,10 @@
       <c r="I43" s="94"/>
     </row>
     <row r="44" spans="1:11" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="125">
+      <c r="A44" s="126">
         <v>2</v>
       </c>
-      <c r="B44" s="135"/>
+      <c r="B44" s="122"/>
       <c r="C44" s="21">
         <f>I42 + 1</f>
         <v>28</v>
@@ -2843,8 +2842,8 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="127"/>
-      <c r="B45" s="135"/>
+      <c r="A45" s="129"/>
+      <c r="B45" s="122"/>
       <c r="C45" s="107"/>
       <c r="D45" s="102" t="s">
         <v>41</v>
@@ -2860,11 +2859,11 @@
       <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="126">
+      <c r="A46" s="128">
         <f>A49 + 1</f>
         <v>1</v>
       </c>
-      <c r="B46" s="129" t="s">
+      <c r="B46" s="123" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="41">
@@ -2897,8 +2896,8 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="125"/>
-      <c r="B47" s="130"/>
+      <c r="A47" s="126"/>
+      <c r="B47" s="124"/>
       <c r="C47" s="42"/>
       <c r="D47" s="7" t="s">
         <v>7</v>
@@ -2910,14 +2909,14 @@
       <c r="G47" s="49"/>
       <c r="H47" s="8"/>
       <c r="I47" s="51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="137">
+      <c r="A48" s="130">
         <v>0</v>
       </c>
-      <c r="B48" s="130"/>
+      <c r="B48" s="124"/>
       <c r="C48" s="25">
         <f>I46 + 1</f>
         <v>12</v>
@@ -2948,17 +2947,17 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="138.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="138"/>
-      <c r="B49" s="136"/>
+      <c r="A49" s="131"/>
+      <c r="B49" s="125"/>
       <c r="C49" s="12"/>
       <c r="D49" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E49" s="75" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F49" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G49" s="26"/>
       <c r="H49" s="12"/>
@@ -2967,6 +2966,19 @@
     <row r="50" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B14"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B29:B35"/>
     <mergeCell ref="B38:B45"/>
     <mergeCell ref="B46:B49"/>
     <mergeCell ref="A13:A14"/>
@@ -2980,19 +2992,6 @@
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B14"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B29:B35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated due date for assign06
</commit_message>
<xml_diff>
--- a/CS320-Spring2019Calendar.xlsx
+++ b/CS320-Spring2019Calendar.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\djhake2\cs320-spring2019\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="90" yWindow="-165" windowWidth="20595" windowHeight="13905"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="75">
   <si>
     <t>Monday</t>
   </si>
@@ -409,12 +414,15 @@
 A SNOW DAY
 (you're never too old to enjoy a snow day…  :-)</t>
   </si>
+  <si>
+    <t>A06: Domain Analysis due</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -497,6 +505,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1027,7 +1043,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1389,62 +1405,65 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1506,7 +1525,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1541,7 +1560,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1752,8 +1771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,17 +1790,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="121" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="133"/>
-      <c r="C1" s="133"/>
-      <c r="D1" s="133"/>
-      <c r="E1" s="133"/>
-      <c r="F1" s="133"/>
-      <c r="G1" s="133"/>
-      <c r="H1" s="133"/>
-      <c r="I1" s="134"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="123"/>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1811,10 +1830,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="128">
+      <c r="A3" s="127">
         <v>16</v>
       </c>
-      <c r="B3" s="123" t="s">
+      <c r="B3" s="130" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="55">
@@ -1847,7 +1866,7 @@
     </row>
     <row r="4" spans="1:13" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="126"/>
-      <c r="B4" s="124"/>
+      <c r="B4" s="131"/>
       <c r="C4" s="53" t="s">
         <v>8</v>
       </c>
@@ -1870,7 +1889,7 @@
       <c r="A5" s="126">
         <v>15</v>
       </c>
-      <c r="B5" s="124"/>
+      <c r="B5" s="131"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>27</v>
@@ -1900,8 +1919,8 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="129"/>
-      <c r="B6" s="124"/>
+      <c r="A6" s="128"/>
+      <c r="B6" s="131"/>
       <c r="C6" s="88" t="s">
         <v>56</v>
       </c>
@@ -1923,10 +1942,10 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="128">
+      <c r="A7" s="127">
         <v>14</v>
       </c>
-      <c r="B7" s="137" t="s">
+      <c r="B7" s="132" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="91">
@@ -1959,8 +1978,8 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="127"/>
-      <c r="B8" s="138"/>
+      <c r="A8" s="129"/>
+      <c r="B8" s="133"/>
       <c r="C8" s="52" t="s">
         <v>57</v>
       </c>
@@ -1980,10 +1999,10 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="136">
+      <c r="A9" s="125">
         <v>13</v>
       </c>
-      <c r="B9" s="138"/>
+      <c r="B9" s="133"/>
       <c r="C9" s="18">
         <f>I7 + 1</f>
         <v>10</v>
@@ -2015,7 +2034,7 @@
     </row>
     <row r="10" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="126"/>
-      <c r="B10" s="138"/>
+      <c r="B10" s="133"/>
       <c r="C10" s="52" t="s">
         <v>59</v>
       </c>
@@ -2036,7 +2055,7 @@
       <c r="A11" s="126">
         <v>12</v>
       </c>
-      <c r="B11" s="138"/>
+      <c r="B11" s="133"/>
       <c r="C11" s="21">
         <f>I9 + 1</f>
         <v>17</v>
@@ -2068,7 +2087,7 @@
     </row>
     <row r="12" spans="1:13" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="126"/>
-      <c r="B12" s="138"/>
+      <c r="B12" s="133"/>
       <c r="C12" s="52" t="s">
         <v>71</v>
       </c>
@@ -2089,7 +2108,7 @@
       <c r="A13" s="126">
         <v>11</v>
       </c>
-      <c r="B13" s="138"/>
+      <c r="B13" s="133"/>
       <c r="C13" s="21">
         <f>I11 + 1</f>
         <v>24</v>
@@ -2119,8 +2138,8 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="127"/>
-      <c r="B14" s="138"/>
+      <c r="A14" s="129"/>
+      <c r="B14" s="133"/>
       <c r="C14" s="96"/>
       <c r="D14" s="44" t="s">
         <v>19</v>
@@ -2140,10 +2159,10 @@
       <c r="M14" s="38"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="128">
+      <c r="A15" s="127">
         <v>10</v>
       </c>
-      <c r="B15" s="137" t="s">
+      <c r="B15" s="132" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="55">
@@ -2176,17 +2195,16 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="129"/>
-      <c r="B16" s="139"/>
+      <c r="A16" s="128"/>
+      <c r="B16" s="134"/>
       <c r="C16" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="61" t="str">
-        <f t="shared" ref="D16:I16" si="2">C16</f>
-        <v>WINTER BREAK</v>
+      <c r="D16" s="140" t="s">
+        <v>74</v>
       </c>
       <c r="E16" s="62" t="str">
-        <f t="shared" si="2"/>
+        <f>C16</f>
         <v>WINTER BREAK</v>
       </c>
       <c r="F16" s="64" t="str">
@@ -2202,7 +2220,7 @@
         <v>WINTER BREAK</v>
       </c>
       <c r="I16" s="63" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D16:I16" si="2">H16</f>
         <v>WINTER BREAK</v>
       </c>
     </row>
@@ -2313,19 +2331,19 @@
       <c r="I25" s="30"/>
     </row>
     <row r="26" spans="1:11" s="32" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="132" t="str">
+      <c r="A26" s="121" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2019 Schedule
 (as of 2-20-2019, subject to change)</v>
       </c>
-      <c r="B26" s="133"/>
-      <c r="C26" s="133"/>
-      <c r="D26" s="133"/>
-      <c r="E26" s="133"/>
-      <c r="F26" s="133"/>
-      <c r="G26" s="133"/>
-      <c r="H26" s="133"/>
-      <c r="I26" s="134"/>
+      <c r="B26" s="122"/>
+      <c r="C26" s="122"/>
+      <c r="D26" s="122"/>
+      <c r="E26" s="122"/>
+      <c r="F26" s="122"/>
+      <c r="G26" s="122"/>
+      <c r="H26" s="122"/>
+      <c r="I26" s="123"/>
     </row>
     <row r="27" spans="1:11" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
@@ -2363,7 +2381,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="135">
+      <c r="A28" s="124">
         <v>10</v>
       </c>
       <c r="B28" s="80"/>
@@ -2397,8 +2415,8 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="136"/>
-      <c r="B29" s="124" t="s">
+      <c r="A29" s="125"/>
+      <c r="B29" s="131" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="101" t="s">
@@ -2430,10 +2448,10 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="136">
+      <c r="A30" s="125">
         <v>9</v>
       </c>
-      <c r="B30" s="124"/>
+      <c r="B30" s="131"/>
       <c r="C30" s="100">
         <f>I15 + 1</f>
         <v>10</v>
@@ -2465,7 +2483,7 @@
     </row>
     <row r="31" spans="1:11" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="126"/>
-      <c r="B31" s="124"/>
+      <c r="B31" s="131"/>
       <c r="C31" s="53" t="str">
         <f>I29</f>
         <v>WINTER BREAK</v>
@@ -2492,7 +2510,7 @@
       <c r="A32" s="126">
         <v>8</v>
       </c>
-      <c r="B32" s="124"/>
+      <c r="B32" s="131"/>
       <c r="C32" s="25">
         <f>I30 + 1</f>
         <v>17</v>
@@ -2524,7 +2542,7 @@
     </row>
     <row r="33" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="126"/>
-      <c r="B33" s="124"/>
+      <c r="B33" s="131"/>
       <c r="C33" s="10"/>
       <c r="D33" s="40" t="s">
         <v>42</v>
@@ -2546,7 +2564,7 @@
       <c r="A34" s="126">
         <v>7</v>
       </c>
-      <c r="B34" s="124"/>
+      <c r="B34" s="131"/>
       <c r="C34" s="10">
         <f>I32 + 1</f>
         <v>24</v>
@@ -2578,7 +2596,7 @@
     </row>
     <row r="35" spans="1:11" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="126"/>
-      <c r="B35" s="124"/>
+      <c r="B35" s="131"/>
       <c r="C35" s="10"/>
       <c r="D35" s="102" t="s">
         <v>16</v>
@@ -2627,7 +2645,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="129"/>
+      <c r="A37" s="128"/>
       <c r="B37" s="82"/>
       <c r="C37" s="116"/>
       <c r="D37" s="115" t="s">
@@ -2644,10 +2662,10 @@
       <c r="I37" s="46"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="128">
+      <c r="A38" s="127">
         <v>5</v>
       </c>
-      <c r="B38" s="121" t="s">
+      <c r="B38" s="135" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="48">
@@ -2681,7 +2699,7 @@
     </row>
     <row r="39" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="126"/>
-      <c r="B39" s="122"/>
+      <c r="B39" s="136"/>
       <c r="C39" s="48"/>
       <c r="D39" s="28" t="s">
         <v>39</v>
@@ -2702,7 +2720,7 @@
       <c r="A40" s="126">
         <v>4</v>
       </c>
-      <c r="B40" s="122"/>
+      <c r="B40" s="136"/>
       <c r="C40" s="21">
         <f>I38 + 1</f>
         <v>14</v>
@@ -2734,7 +2752,7 @@
     </row>
     <row r="41" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="126"/>
-      <c r="B41" s="122"/>
+      <c r="B41" s="136"/>
       <c r="C41" s="47"/>
       <c r="D41" s="108" t="s">
         <v>52</v>
@@ -2759,7 +2777,7 @@
       <c r="A42" s="126">
         <v>3</v>
       </c>
-      <c r="B42" s="122"/>
+      <c r="B42" s="136"/>
       <c r="C42" s="53">
         <f>I40 + 1</f>
         <v>21</v>
@@ -2791,7 +2809,7 @@
     </row>
     <row r="43" spans="1:11" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="126"/>
-      <c r="B43" s="122"/>
+      <c r="B43" s="136"/>
       <c r="C43" s="53" t="s">
         <v>6</v>
       </c>
@@ -2812,7 +2830,7 @@
       <c r="A44" s="126">
         <v>2</v>
       </c>
-      <c r="B44" s="122"/>
+      <c r="B44" s="136"/>
       <c r="C44" s="21">
         <f>I42 + 1</f>
         <v>28</v>
@@ -2842,8 +2860,8 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="129"/>
-      <c r="B45" s="122"/>
+      <c r="A45" s="128"/>
+      <c r="B45" s="136"/>
       <c r="C45" s="107"/>
       <c r="D45" s="102" t="s">
         <v>41</v>
@@ -2859,11 +2877,11 @@
       <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="128">
+      <c r="A46" s="127">
         <f>A49 + 1</f>
         <v>1</v>
       </c>
-      <c r="B46" s="123" t="s">
+      <c r="B46" s="130" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="41">
@@ -2897,7 +2915,7 @@
     </row>
     <row r="47" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="126"/>
-      <c r="B47" s="124"/>
+      <c r="B47" s="131"/>
       <c r="C47" s="42"/>
       <c r="D47" s="7" t="s">
         <v>7</v>
@@ -2913,10 +2931,10 @@
       </c>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="130">
+      <c r="A48" s="138">
         <v>0</v>
       </c>
-      <c r="B48" s="124"/>
+      <c r="B48" s="131"/>
       <c r="C48" s="25">
         <f>I46 + 1</f>
         <v>12</v>
@@ -2947,8 +2965,8 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="138.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="131"/>
-      <c r="B49" s="125"/>
+      <c r="A49" s="139"/>
+      <c r="B49" s="137"/>
       <c r="C49" s="12"/>
       <c r="D49" s="29" t="s">
         <v>55</v>
@@ -2966,6 +2984,19 @@
     <row r="50" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B38:B45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A31"/>
@@ -2979,19 +3010,6 @@
     <mergeCell ref="A26:I26"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B29:B35"/>
-    <mergeCell ref="B38:B45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated due date on calendar for assign06
</commit_message>
<xml_diff>
--- a/CS320-Spring2019Calendar.xlsx
+++ b/CS320-Spring2019Calendar.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
   <si>
     <t>Monday</t>
   </si>
@@ -361,11 +361,6 @@
 A11: Team Project
 Final Self/Peer Evaluations due
 both 7:00 am (Marmoset)</t>
-  </si>
-  <si>
-    <t>A06: Team Problem Domain Analysis due
-7:00 am
-(Violet UML &amp; Google Doc)</t>
   </si>
   <si>
     <t>Lab 2: Web Apps I due
@@ -1043,7 +1038,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1405,32 +1400,14 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1438,6 +1415,42 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1447,22 +1460,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1772,7 +1770,7 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,17 +1788,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="121" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
-      <c r="I1" s="123"/>
+      <c r="A1" s="133" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="134"/>
+      <c r="I1" s="135"/>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1830,10 +1828,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="127">
+      <c r="A3" s="129">
         <v>16</v>
       </c>
-      <c r="B3" s="130" t="s">
+      <c r="B3" s="124" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="55">
@@ -1865,8 +1863,8 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="126"/>
-      <c r="B4" s="131"/>
+      <c r="A4" s="127"/>
+      <c r="B4" s="125"/>
       <c r="C4" s="53" t="s">
         <v>8</v>
       </c>
@@ -1886,10 +1884,10 @@
       <c r="I4" s="93"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="126">
+      <c r="A5" s="127">
         <v>15</v>
       </c>
-      <c r="B5" s="131"/>
+      <c r="B5" s="125"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>27</v>
@@ -1919,8 +1917,8 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="128"/>
-      <c r="B6" s="131"/>
+      <c r="A6" s="130"/>
+      <c r="B6" s="125"/>
       <c r="C6" s="88" t="s">
         <v>56</v>
       </c>
@@ -1932,20 +1930,20 @@
         <v>44</v>
       </c>
       <c r="G6" s="83" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H6" s="119" t="s">
         <v>45</v>
       </c>
       <c r="I6" s="51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="127">
+      <c r="A7" s="129">
         <v>14</v>
       </c>
-      <c r="B7" s="132" t="s">
+      <c r="B7" s="138" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="91">
@@ -1978,8 +1976,8 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="129"/>
-      <c r="B8" s="133"/>
+      <c r="A8" s="128"/>
+      <c r="B8" s="139"/>
       <c r="C8" s="52" t="s">
         <v>57</v>
       </c>
@@ -1999,10 +1997,10 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="125">
+      <c r="A9" s="137">
         <v>13</v>
       </c>
-      <c r="B9" s="133"/>
+      <c r="B9" s="139"/>
       <c r="C9" s="18">
         <f>I7 + 1</f>
         <v>10</v>
@@ -2033,8 +2031,8 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="126"/>
-      <c r="B10" s="133"/>
+      <c r="A10" s="127"/>
+      <c r="B10" s="139"/>
       <c r="C10" s="52" t="s">
         <v>59</v>
       </c>
@@ -2052,10 +2050,10 @@
       <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="126">
+      <c r="A11" s="127">
         <v>12</v>
       </c>
-      <c r="B11" s="133"/>
+      <c r="B11" s="139"/>
       <c r="C11" s="21">
         <f>I9 + 1</f>
         <v>17</v>
@@ -2086,17 +2084,17 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="126"/>
-      <c r="B12" s="133"/>
+      <c r="A12" s="127"/>
+      <c r="B12" s="139"/>
       <c r="C12" s="52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D12" s="120" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="44" t="s">
@@ -2105,10 +2103,10 @@
       <c r="I12" s="94"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="126">
+      <c r="A13" s="127">
         <v>11</v>
       </c>
-      <c r="B13" s="133"/>
+      <c r="B13" s="139"/>
       <c r="C13" s="21">
         <f>I11 + 1</f>
         <v>24</v>
@@ -2132,14 +2130,14 @@
       <c r="H13" s="41">
         <v>1</v>
       </c>
-      <c r="I13" s="59">
+      <c r="I13" s="141">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="129"/>
-      <c r="B14" s="133"/>
+      <c r="A14" s="128"/>
+      <c r="B14" s="139"/>
       <c r="C14" s="96"/>
       <c r="D14" s="44" t="s">
         <v>19</v>
@@ -2152,17 +2150,15 @@
       <c r="H14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="51" t="s">
-        <v>67</v>
-      </c>
+      <c r="I14" s="77"/>
       <c r="L14" s="38"/>
       <c r="M14" s="38"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="127">
+      <c r="A15" s="129">
         <v>10</v>
       </c>
-      <c r="B15" s="132" t="s">
+      <c r="B15" s="138" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="55">
@@ -2195,13 +2191,13 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="128"/>
-      <c r="B16" s="134"/>
+      <c r="A16" s="130"/>
+      <c r="B16" s="140"/>
       <c r="C16" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="140" t="s">
-        <v>74</v>
+      <c r="D16" s="121" t="s">
+        <v>73</v>
       </c>
       <c r="E16" s="62" t="str">
         <f>C16</f>
@@ -2220,7 +2216,7 @@
         <v>WINTER BREAK</v>
       </c>
       <c r="I16" s="63" t="str">
-        <f t="shared" ref="D16:I16" si="2">H16</f>
+        <f t="shared" ref="I16" si="2">H16</f>
         <v>WINTER BREAK</v>
       </c>
     </row>
@@ -2331,19 +2327,19 @@
       <c r="I25" s="30"/>
     </row>
     <row r="26" spans="1:11" s="32" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="121" t="str">
+      <c r="A26" s="133" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2019 Schedule
 (as of 2-20-2019, subject to change)</v>
       </c>
-      <c r="B26" s="122"/>
-      <c r="C26" s="122"/>
-      <c r="D26" s="122"/>
-      <c r="E26" s="122"/>
-      <c r="F26" s="122"/>
-      <c r="G26" s="122"/>
-      <c r="H26" s="122"/>
-      <c r="I26" s="123"/>
+      <c r="B26" s="134"/>
+      <c r="C26" s="134"/>
+      <c r="D26" s="134"/>
+      <c r="E26" s="134"/>
+      <c r="F26" s="134"/>
+      <c r="G26" s="134"/>
+      <c r="H26" s="134"/>
+      <c r="I26" s="135"/>
     </row>
     <row r="27" spans="1:11" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
@@ -2381,7 +2377,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="124">
+      <c r="A28" s="136">
         <v>10</v>
       </c>
       <c r="B28" s="80"/>
@@ -2415,8 +2411,8 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="125"/>
-      <c r="B29" s="131" t="s">
+      <c r="A29" s="137"/>
+      <c r="B29" s="125" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="101" t="s">
@@ -2448,10 +2444,10 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="125">
+      <c r="A30" s="137">
         <v>9</v>
       </c>
-      <c r="B30" s="131"/>
+      <c r="B30" s="125"/>
       <c r="C30" s="100">
         <f>I15 + 1</f>
         <v>10</v>
@@ -2482,8 +2478,8 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="126"/>
-      <c r="B31" s="131"/>
+      <c r="A31" s="127"/>
+      <c r="B31" s="125"/>
       <c r="C31" s="53" t="str">
         <f>I29</f>
         <v>WINTER BREAK</v>
@@ -2507,10 +2503,10 @@
       <c r="K31" s="39"/>
     </row>
     <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="126">
+      <c r="A32" s="127">
         <v>8</v>
       </c>
-      <c r="B32" s="131"/>
+      <c r="B32" s="125"/>
       <c r="C32" s="25">
         <f>I30 + 1</f>
         <v>17</v>
@@ -2541,8 +2537,8 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="126"/>
-      <c r="B33" s="131"/>
+      <c r="A33" s="127"/>
+      <c r="B33" s="125"/>
       <c r="C33" s="10"/>
       <c r="D33" s="40" t="s">
         <v>42</v>
@@ -2561,10 +2557,10 @@
       <c r="K33" s="37"/>
     </row>
     <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="126">
+      <c r="A34" s="127">
         <v>7</v>
       </c>
-      <c r="B34" s="131"/>
+      <c r="B34" s="125"/>
       <c r="C34" s="10">
         <f>I32 + 1</f>
         <v>24</v>
@@ -2595,8 +2591,8 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="126"/>
-      <c r="B35" s="131"/>
+      <c r="A35" s="127"/>
+      <c r="B35" s="125"/>
       <c r="C35" s="10"/>
       <c r="D35" s="102" t="s">
         <v>16</v>
@@ -2612,7 +2608,7 @@
       <c r="I35" s="77"/>
     </row>
     <row r="36" spans="1:11" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="126">
+      <c r="A36" s="127">
         <v>6</v>
       </c>
       <c r="B36" s="81"/>
@@ -2645,7 +2641,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="128"/>
+      <c r="A37" s="130"/>
       <c r="B37" s="82"/>
       <c r="C37" s="116"/>
       <c r="D37" s="115" t="s">
@@ -2662,10 +2658,10 @@
       <c r="I37" s="46"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="127">
+      <c r="A38" s="129">
         <v>5</v>
       </c>
-      <c r="B38" s="135" t="s">
+      <c r="B38" s="122" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="48">
@@ -2698,8 +2694,8 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="126"/>
-      <c r="B39" s="136"/>
+      <c r="A39" s="127"/>
+      <c r="B39" s="123"/>
       <c r="C39" s="48"/>
       <c r="D39" s="28" t="s">
         <v>39</v>
@@ -2717,10 +2713,10 @@
       <c r="I39" s="78"/>
     </row>
     <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="126">
+      <c r="A40" s="127">
         <v>4</v>
       </c>
-      <c r="B40" s="136"/>
+      <c r="B40" s="123"/>
       <c r="C40" s="21">
         <f>I38 + 1</f>
         <v>14</v>
@@ -2751,8 +2747,8 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="126"/>
-      <c r="B41" s="136"/>
+      <c r="A41" s="127"/>
+      <c r="B41" s="123"/>
       <c r="C41" s="47"/>
       <c r="D41" s="108" t="s">
         <v>52</v>
@@ -2774,10 +2770,10 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="126">
+      <c r="A42" s="127">
         <v>3</v>
       </c>
-      <c r="B42" s="136"/>
+      <c r="B42" s="123"/>
       <c r="C42" s="53">
         <f>I40 + 1</f>
         <v>21</v>
@@ -2808,8 +2804,8 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="126"/>
-      <c r="B43" s="136"/>
+      <c r="A43" s="127"/>
+      <c r="B43" s="123"/>
       <c r="C43" s="53" t="s">
         <v>6</v>
       </c>
@@ -2827,10 +2823,10 @@
       <c r="I43" s="94"/>
     </row>
     <row r="44" spans="1:11" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="126">
+      <c r="A44" s="127">
         <v>2</v>
       </c>
-      <c r="B44" s="136"/>
+      <c r="B44" s="123"/>
       <c r="C44" s="21">
         <f>I42 + 1</f>
         <v>28</v>
@@ -2860,8 +2856,8 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="128"/>
-      <c r="B45" s="136"/>
+      <c r="A45" s="130"/>
+      <c r="B45" s="123"/>
       <c r="C45" s="107"/>
       <c r="D45" s="102" t="s">
         <v>41</v>
@@ -2877,11 +2873,11 @@
       <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="127">
+      <c r="A46" s="129">
         <f>A49 + 1</f>
         <v>1</v>
       </c>
-      <c r="B46" s="130" t="s">
+      <c r="B46" s="124" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="41">
@@ -2914,8 +2910,8 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="126"/>
-      <c r="B47" s="131"/>
+      <c r="A47" s="127"/>
+      <c r="B47" s="125"/>
       <c r="C47" s="42"/>
       <c r="D47" s="7" t="s">
         <v>7</v>
@@ -2931,10 +2927,10 @@
       </c>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="138">
+      <c r="A48" s="131">
         <v>0</v>
       </c>
-      <c r="B48" s="131"/>
+      <c r="B48" s="125"/>
       <c r="C48" s="25">
         <f>I46 + 1</f>
         <v>12</v>
@@ -2965,8 +2961,8 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="138.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="139"/>
-      <c r="B49" s="137"/>
+      <c r="A49" s="132"/>
+      <c r="B49" s="126"/>
       <c r="C49" s="12"/>
       <c r="D49" s="29" t="s">
         <v>55</v>
@@ -2984,6 +2980,19 @@
     <row r="50" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B14"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B29:B35"/>
     <mergeCell ref="B38:B45"/>
     <mergeCell ref="B46:B49"/>
     <mergeCell ref="A13:A14"/>
@@ -2997,19 +3006,6 @@
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B14"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B29:B35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
change lab04 due date
</commit_message>
<xml_diff>
--- a/CS320-Spring2019Calendar.xlsx
+++ b/CS320-Spring2019Calendar.xlsx
@@ -148,24 +148,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Lecture 14: DB Applications, JDBC
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lab 5: JDBC
-(assigned)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Lecture  15: ORM, Designing a Persistence Layer
 </t>
     </r>
@@ -325,11 +307,6 @@
   </si>
   <si>
     <t>Lab 2a: Web Apps II due
-7:00 am
-(Marmoset)</t>
-  </si>
-  <si>
-    <t>Lab 4: SQL due
 7:00 am
 (Marmoset)</t>
   </si>
@@ -401,16 +378,64 @@
 (Google Doc)</t>
   </si>
   <si>
-    <t>CS320: SW Engineering - Spring 2019 Schedule
-(as of 2-20-2019, subject to change)</t>
-  </si>
-  <si>
     <t>WOO…! HOO…!
 A SNOW DAY
 (you're never too old to enjoy a snow day…  :-)</t>
   </si>
   <si>
     <t>A06: Domain Analysis due</t>
+  </si>
+  <si>
+    <t>Lab 4: SQL due
+7:00 am
+WEDS, 3-13 --&gt;
+(Marmoset)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lecture 14: DB Applications, JDBC
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lab 4: SQL
+due (7:00a)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lab 5: JDBC
+(assigned)</t>
+    </r>
+  </si>
+  <si>
+    <t>CS320: SW Engineering - Spring 2019 Schedule
+(as of 3-11-2019, subject to change)</t>
   </si>
 </sst>
 </file>
@@ -1403,64 +1428,64 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1769,8 +1794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1788,21 +1813,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="133" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="135"/>
+      <c r="A1" s="123" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="125"/>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
@@ -1831,7 +1856,7 @@
       <c r="A3" s="129">
         <v>16</v>
       </c>
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="132" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="55">
@@ -1863,8 +1888,8 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="127"/>
-      <c r="B4" s="125"/>
+      <c r="A4" s="128"/>
+      <c r="B4" s="133"/>
       <c r="C4" s="53" t="s">
         <v>8</v>
       </c>
@@ -1884,10 +1909,10 @@
       <c r="I4" s="93"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="127">
+      <c r="A5" s="128">
         <v>15</v>
       </c>
-      <c r="B5" s="125"/>
+      <c r="B5" s="133"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>27</v>
@@ -1918,32 +1943,32 @@
     </row>
     <row r="6" spans="1:13" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="130"/>
-      <c r="B6" s="125"/>
+      <c r="B6" s="133"/>
       <c r="C6" s="88" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="89" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="90"/>
       <c r="F6" s="89" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="83" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="83" t="s">
-        <v>67</v>
-      </c>
-      <c r="H6" s="119" t="s">
-        <v>45</v>
-      </c>
       <c r="I6" s="51" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="129">
         <v>14</v>
       </c>
-      <c r="B7" s="138" t="s">
+      <c r="B7" s="134" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="91">
@@ -1976,31 +2001,31 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="128"/>
-      <c r="B8" s="139"/>
+      <c r="A8" s="131"/>
+      <c r="B8" s="135"/>
       <c r="C8" s="52" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" s="79" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="87"/>
       <c r="F8" s="79" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G8" s="86"/>
       <c r="H8" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I8" s="51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="137">
+      <c r="A9" s="127">
         <v>13</v>
       </c>
-      <c r="B9" s="139"/>
+      <c r="B9" s="135"/>
       <c r="C9" s="18">
         <f>I7 + 1</f>
         <v>10</v>
@@ -2031,29 +2056,29 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="127"/>
-      <c r="B10" s="139"/>
+      <c r="A10" s="128"/>
+      <c r="B10" s="135"/>
       <c r="C10" s="52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="127">
+      <c r="A11" s="128">
         <v>12</v>
       </c>
-      <c r="B11" s="139"/>
+      <c r="B11" s="135"/>
       <c r="C11" s="21">
         <f>I9 + 1</f>
         <v>17</v>
@@ -2084,29 +2109,29 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="127"/>
-      <c r="B12" s="139"/>
+      <c r="A12" s="128"/>
+      <c r="B12" s="135"/>
       <c r="C12" s="52" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D12" s="120" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I12" s="94"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="127">
+      <c r="A13" s="128">
         <v>11</v>
       </c>
-      <c r="B13" s="139"/>
+      <c r="B13" s="135"/>
       <c r="C13" s="21">
         <f>I11 + 1</f>
         <v>24</v>
@@ -2130,14 +2155,14 @@
       <c r="H13" s="41">
         <v>1</v>
       </c>
-      <c r="I13" s="141">
+      <c r="I13" s="122">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="128"/>
-      <c r="B14" s="139"/>
+      <c r="A14" s="131"/>
+      <c r="B14" s="135"/>
       <c r="C14" s="96"/>
       <c r="D14" s="44" t="s">
         <v>19</v>
@@ -2158,7 +2183,7 @@
       <c r="A15" s="129">
         <v>10</v>
       </c>
-      <c r="B15" s="138" t="s">
+      <c r="B15" s="134" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="55">
@@ -2192,12 +2217,12 @@
     </row>
     <row r="16" spans="1:13" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="130"/>
-      <c r="B16" s="140"/>
+      <c r="B16" s="136"/>
       <c r="C16" s="60" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="121" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E16" s="62" t="str">
         <f>C16</f>
@@ -2236,7 +2261,7 @@
       <c r="B18" s="31"/>
       <c r="D18" s="34"/>
       <c r="E18" s="76" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="34"/>
@@ -2248,7 +2273,7 @@
       <c r="B19" s="36"/>
       <c r="D19" s="30"/>
       <c r="E19" s="70" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
@@ -2260,7 +2285,7 @@
       <c r="B20" s="31"/>
       <c r="D20" s="34"/>
       <c r="E20" s="71" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="34"/>
@@ -2272,7 +2297,7 @@
       <c r="B21" s="31"/>
       <c r="D21" s="34"/>
       <c r="E21" s="72" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="34"/>
@@ -2284,7 +2309,7 @@
       <c r="B22" s="31"/>
       <c r="D22" s="34"/>
       <c r="E22" s="73" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="34"/>
@@ -2297,7 +2322,7 @@
       <c r="C23" s="68"/>
       <c r="D23" s="34"/>
       <c r="E23" s="74" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="34"/>
@@ -2327,19 +2352,19 @@
       <c r="I25" s="30"/>
     </row>
     <row r="26" spans="1:11" s="32" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="133" t="str">
+      <c r="A26" s="123" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2019 Schedule
-(as of 2-20-2019, subject to change)</v>
-      </c>
-      <c r="B26" s="134"/>
-      <c r="C26" s="134"/>
-      <c r="D26" s="134"/>
-      <c r="E26" s="134"/>
-      <c r="F26" s="134"/>
-      <c r="G26" s="134"/>
-      <c r="H26" s="134"/>
-      <c r="I26" s="135"/>
+(as of 3-11-2019, subject to change)</v>
+      </c>
+      <c r="B26" s="124"/>
+      <c r="C26" s="124"/>
+      <c r="D26" s="124"/>
+      <c r="E26" s="124"/>
+      <c r="F26" s="124"/>
+      <c r="G26" s="124"/>
+      <c r="H26" s="124"/>
+      <c r="I26" s="125"/>
     </row>
     <row r="27" spans="1:11" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
@@ -2377,7 +2402,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="136">
+      <c r="A28" s="126">
         <v>10</v>
       </c>
       <c r="B28" s="80"/>
@@ -2411,12 +2436,12 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="137"/>
-      <c r="B29" s="125" t="s">
+      <c r="A29" s="127"/>
+      <c r="B29" s="133" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="101" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D29" s="54" t="str">
         <f t="shared" ref="D29" si="5">C29</f>
@@ -2444,10 +2469,10 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="137">
+      <c r="A30" s="127">
         <v>9</v>
       </c>
-      <c r="B30" s="125"/>
+      <c r="B30" s="133"/>
       <c r="C30" s="100">
         <f>I15 + 1</f>
         <v>10</v>
@@ -2478,8 +2503,8 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="127"/>
-      <c r="B31" s="125"/>
+      <c r="A31" s="128"/>
+      <c r="B31" s="133"/>
       <c r="C31" s="53" t="str">
         <f>I29</f>
         <v>WINTER BREAK</v>
@@ -2488,25 +2513,25 @@
         <v>26</v>
       </c>
       <c r="E31" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>27</v>
+        <v>71</v>
+      </c>
+      <c r="F31" s="120" t="s">
+        <v>72</v>
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I31" s="51" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K31" s="39"/>
     </row>
     <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="127">
+      <c r="A32" s="128">
         <v>8</v>
       </c>
-      <c r="B32" s="125"/>
+      <c r="B32" s="133"/>
       <c r="C32" s="25">
         <f>I30 + 1</f>
         <v>17</v>
@@ -2537,30 +2562,30 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="127"/>
-      <c r="B33" s="125"/>
+      <c r="A33" s="128"/>
+      <c r="B33" s="133"/>
       <c r="C33" s="10"/>
       <c r="D33" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G33" s="7"/>
       <c r="H33" s="7" t="s">
         <v>22</v>
       </c>
       <c r="I33" s="51" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K33" s="37"/>
     </row>
     <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="127">
+      <c r="A34" s="128">
         <v>7</v>
       </c>
-      <c r="B34" s="125"/>
+      <c r="B34" s="133"/>
       <c r="C34" s="10">
         <f>I32 + 1</f>
         <v>24</v>
@@ -2591,8 +2616,8 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="127"/>
-      <c r="B35" s="125"/>
+      <c r="A35" s="128"/>
+      <c r="B35" s="133"/>
       <c r="C35" s="10"/>
       <c r="D35" s="102" t="s">
         <v>16</v>
@@ -2603,12 +2628,12 @@
       </c>
       <c r="G35" s="90"/>
       <c r="H35" s="89" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I35" s="77"/>
     </row>
     <row r="36" spans="1:11" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="127">
+      <c r="A36" s="128">
         <v>6</v>
       </c>
       <c r="B36" s="81"/>
@@ -2645,7 +2670,7 @@
       <c r="B37" s="82"/>
       <c r="C37" s="116"/>
       <c r="D37" s="115" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E37" s="87"/>
       <c r="F37" s="79" t="s">
@@ -2661,7 +2686,7 @@
       <c r="A38" s="129">
         <v>5</v>
       </c>
-      <c r="B38" s="122" t="s">
+      <c r="B38" s="137" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="48">
@@ -2694,29 +2719,29 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="127"/>
-      <c r="B39" s="123"/>
+      <c r="A39" s="128"/>
+      <c r="B39" s="138"/>
       <c r="C39" s="48"/>
       <c r="D39" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E39" s="117" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F39" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G39" s="15"/>
       <c r="H39" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I39" s="78"/>
     </row>
     <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="127">
+      <c r="A40" s="128">
         <v>4</v>
       </c>
-      <c r="B40" s="123"/>
+      <c r="B40" s="138"/>
       <c r="C40" s="21">
         <f>I38 + 1</f>
         <v>14</v>
@@ -2747,17 +2772,17 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="127"/>
-      <c r="B41" s="123"/>
+      <c r="A41" s="128"/>
+      <c r="B41" s="138"/>
       <c r="C41" s="47"/>
       <c r="D41" s="108" t="s">
+        <v>51</v>
+      </c>
+      <c r="E41" s="106" t="s">
+        <v>62</v>
+      </c>
+      <c r="F41" s="112" t="s">
         <v>52</v>
-      </c>
-      <c r="E41" s="106" t="s">
-        <v>64</v>
-      </c>
-      <c r="F41" s="112" t="s">
-        <v>53</v>
       </c>
       <c r="G41" s="57" t="s">
         <v>6</v>
@@ -2770,10 +2795,10 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="127">
+      <c r="A42" s="128">
         <v>3</v>
       </c>
-      <c r="B42" s="123"/>
+      <c r="B42" s="138"/>
       <c r="C42" s="53">
         <f>I40 + 1</f>
         <v>21</v>
@@ -2804,8 +2829,8 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="127"/>
-      <c r="B43" s="123"/>
+      <c r="A43" s="128"/>
+      <c r="B43" s="138"/>
       <c r="C43" s="53" t="s">
         <v>6</v>
       </c>
@@ -2814,7 +2839,7 @@
       </c>
       <c r="E43" s="15"/>
       <c r="F43" s="105" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G43" s="97"/>
       <c r="H43" s="105" t="s">
@@ -2823,10 +2848,10 @@
       <c r="I43" s="94"/>
     </row>
     <row r="44" spans="1:11" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="127">
+      <c r="A44" s="128">
         <v>2</v>
       </c>
-      <c r="B44" s="123"/>
+      <c r="B44" s="138"/>
       <c r="C44" s="21">
         <f>I42 + 1</f>
         <v>28</v>
@@ -2857,10 +2882,10 @@
     </row>
     <row r="45" spans="1:11" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="130"/>
-      <c r="B45" s="123"/>
+      <c r="B45" s="138"/>
       <c r="C45" s="107"/>
       <c r="D45" s="102" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E45" s="114"/>
       <c r="F45" s="10" t="s">
@@ -2877,7 +2902,7 @@
         <f>A49 + 1</f>
         <v>1</v>
       </c>
-      <c r="B46" s="124" t="s">
+      <c r="B46" s="132" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="41">
@@ -2910,8 +2935,8 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="127"/>
-      <c r="B47" s="125"/>
+      <c r="A47" s="128"/>
+      <c r="B47" s="133"/>
       <c r="C47" s="42"/>
       <c r="D47" s="7" t="s">
         <v>7</v>
@@ -2923,14 +2948,14 @@
       <c r="G47" s="49"/>
       <c r="H47" s="8"/>
       <c r="I47" s="51" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="131">
+      <c r="A48" s="140">
         <v>0</v>
       </c>
-      <c r="B48" s="125"/>
+      <c r="B48" s="133"/>
       <c r="C48" s="25">
         <f>I46 + 1</f>
         <v>12</v>
@@ -2961,17 +2986,17 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="138.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="132"/>
-      <c r="B49" s="126"/>
+      <c r="A49" s="141"/>
+      <c r="B49" s="139"/>
       <c r="C49" s="12"/>
       <c r="D49" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E49" s="75" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F49" s="29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G49" s="26"/>
       <c r="H49" s="12"/>
@@ -2980,6 +3005,19 @@
     <row r="50" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B38:B45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A31"/>
@@ -2993,19 +3031,6 @@
     <mergeCell ref="A26:I26"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B29:B35"/>
-    <mergeCell ref="B38:B45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated schedule and calendar
</commit_message>
<xml_diff>
--- a/CS320-Spring2019Calendar.xlsx
+++ b/CS320-Spring2019Calendar.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\djhake2\cs320-spring2019\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="90" yWindow="-165" windowWidth="20595" windowHeight="13905"/>
   </bookViews>
@@ -16,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="76">
   <si>
     <t>Monday</t>
   </si>
@@ -274,9 +269,6 @@
   </si>
   <si>
     <t>A04: Individual MS3 Final Project Demo</t>
-  </si>
-  <si>
-    <t>TBD</t>
   </si>
   <si>
     <t>FINAL EXAM PERIOD
@@ -446,7 +438,11 @@
   </si>
   <si>
     <t>CS320: SW Engineering - Spring 2019 Schedule
-(as of 3-22-2019, subject to change)</t>
+(as of 4-3-2019, subject to change)</t>
+  </si>
+  <si>
+    <t>Library Example Review
+(in-class)</t>
   </si>
 </sst>
 </file>
@@ -1074,7 +1070,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1409,9 +1405,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1442,32 +1435,11 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1475,6 +1447,42 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1483,21 +1491,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1559,7 +1552,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1594,7 +1587,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1805,8 +1798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1824,17 +1817,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="123" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="124"/>
-      <c r="I1" s="125"/>
+      <c r="A1" s="133" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="134"/>
+      <c r="I1" s="135"/>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1867,7 +1860,7 @@
       <c r="A3" s="129">
         <v>16</v>
       </c>
-      <c r="B3" s="132" t="s">
+      <c r="B3" s="124" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="55">
@@ -1899,8 +1892,8 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="128"/>
-      <c r="B4" s="133"/>
+      <c r="A4" s="127"/>
+      <c r="B4" s="125"/>
       <c r="C4" s="53" t="s">
         <v>8</v>
       </c>
@@ -1920,10 +1913,10 @@
       <c r="I4" s="93"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="128">
+      <c r="A5" s="127">
         <v>15</v>
       </c>
-      <c r="B5" s="133"/>
+      <c r="B5" s="125"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>27</v>
@@ -1947,16 +1940,16 @@
       <c r="H5" s="91">
         <v>1</v>
       </c>
-      <c r="I5" s="118">
+      <c r="I5" s="117">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="130"/>
-      <c r="B6" s="133"/>
+      <c r="B6" s="125"/>
       <c r="C6" s="88" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" s="89" t="s">
         <v>42</v>
@@ -1966,20 +1959,20 @@
         <v>43</v>
       </c>
       <c r="G6" s="83" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="118" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="51" t="s">
         <v>65</v>
-      </c>
-      <c r="H6" s="119" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" s="51" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="129">
         <v>14</v>
       </c>
-      <c r="B7" s="134" t="s">
+      <c r="B7" s="138" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="91">
@@ -2012,10 +2005,10 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="131"/>
-      <c r="B8" s="135"/>
+      <c r="A8" s="128"/>
+      <c r="B8" s="139"/>
       <c r="C8" s="52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="79" t="s">
         <v>34</v>
@@ -2029,14 +2022,14 @@
         <v>47</v>
       </c>
       <c r="I8" s="51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="127">
+      <c r="A9" s="137">
         <v>13</v>
       </c>
-      <c r="B9" s="135"/>
+      <c r="B9" s="139"/>
       <c r="C9" s="18">
         <f>I7 + 1</f>
         <v>10</v>
@@ -2067,10 +2060,10 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="128"/>
-      <c r="B10" s="135"/>
+      <c r="A10" s="127"/>
+      <c r="B10" s="139"/>
       <c r="C10" s="52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>46</v>
@@ -2086,10 +2079,10 @@
       <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="128">
+      <c r="A11" s="127">
         <v>12</v>
       </c>
-      <c r="B11" s="135"/>
+      <c r="B11" s="139"/>
       <c r="C11" s="21">
         <f>I9 + 1</f>
         <v>17</v>
@@ -2120,17 +2113,17 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="128"/>
-      <c r="B12" s="135"/>
+      <c r="A12" s="127"/>
+      <c r="B12" s="139"/>
       <c r="C12" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="120" t="s">
         <v>67</v>
+      </c>
+      <c r="D12" s="119" t="s">
+        <v>66</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="44" t="s">
@@ -2139,10 +2132,10 @@
       <c r="I12" s="94"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="128">
+      <c r="A13" s="127">
         <v>11</v>
       </c>
-      <c r="B13" s="135"/>
+      <c r="B13" s="139"/>
       <c r="C13" s="21">
         <f>I11 + 1</f>
         <v>24</v>
@@ -2166,14 +2159,14 @@
       <c r="H13" s="41">
         <v>1</v>
       </c>
-      <c r="I13" s="122">
+      <c r="I13" s="121">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="131"/>
-      <c r="B14" s="135"/>
+      <c r="A14" s="128"/>
+      <c r="B14" s="139"/>
       <c r="C14" s="96"/>
       <c r="D14" s="44" t="s">
         <v>19</v>
@@ -2194,7 +2187,7 @@
       <c r="A15" s="129">
         <v>10</v>
       </c>
-      <c r="B15" s="134" t="s">
+      <c r="B15" s="138" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="55">
@@ -2228,12 +2221,12 @@
     </row>
     <row r="16" spans="1:13" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="130"/>
-      <c r="B16" s="136"/>
+      <c r="B16" s="140"/>
       <c r="C16" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="121" t="s">
-        <v>70</v>
+      <c r="D16" s="120" t="s">
+        <v>69</v>
       </c>
       <c r="E16" s="62" t="str">
         <f>C16</f>
@@ -2363,19 +2356,19 @@
       <c r="I25" s="30"/>
     </row>
     <row r="26" spans="1:11" s="32" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="123" t="str">
+      <c r="A26" s="133" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2019 Schedule
-(as of 3-22-2019, subject to change)</v>
-      </c>
-      <c r="B26" s="124"/>
-      <c r="C26" s="124"/>
-      <c r="D26" s="124"/>
-      <c r="E26" s="124"/>
-      <c r="F26" s="124"/>
-      <c r="G26" s="124"/>
-      <c r="H26" s="124"/>
-      <c r="I26" s="125"/>
+(as of 4-3-2019, subject to change)</v>
+      </c>
+      <c r="B26" s="134"/>
+      <c r="C26" s="134"/>
+      <c r="D26" s="134"/>
+      <c r="E26" s="134"/>
+      <c r="F26" s="134"/>
+      <c r="G26" s="134"/>
+      <c r="H26" s="134"/>
+      <c r="I26" s="135"/>
     </row>
     <row r="27" spans="1:11" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
@@ -2413,7 +2406,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="126">
+      <c r="A28" s="136">
         <v>10</v>
       </c>
       <c r="B28" s="80"/>
@@ -2447,8 +2440,8 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="127"/>
-      <c r="B29" s="133" t="s">
+      <c r="A29" s="137"/>
+      <c r="B29" s="125" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="101" t="s">
@@ -2480,10 +2473,10 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="127">
+      <c r="A30" s="137">
         <v>9</v>
       </c>
-      <c r="B30" s="133"/>
+      <c r="B30" s="125"/>
       <c r="C30" s="100">
         <f>I15 + 1</f>
         <v>10</v>
@@ -2514,8 +2507,8 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="128"/>
-      <c r="B31" s="133"/>
+      <c r="A31" s="127"/>
+      <c r="B31" s="125"/>
       <c r="C31" s="53" t="str">
         <f>I29</f>
         <v>WINTER BREAK</v>
@@ -2524,25 +2517,25 @@
         <v>26</v>
       </c>
       <c r="E31" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="F31" s="119" t="s">
         <v>71</v>
-      </c>
-      <c r="F31" s="120" t="s">
-        <v>72</v>
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="7" t="s">
         <v>27</v>
       </c>
       <c r="I31" s="51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K31" s="39"/>
     </row>
     <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="128">
+      <c r="A32" s="127">
         <v>8</v>
       </c>
-      <c r="B32" s="133"/>
+      <c r="B32" s="125"/>
       <c r="C32" s="25">
         <f>I30 + 1</f>
         <v>17</v>
@@ -2573,8 +2566,8 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="128"/>
-      <c r="B33" s="133"/>
+      <c r="A33" s="127"/>
+      <c r="B33" s="125"/>
       <c r="C33" s="10"/>
       <c r="D33" s="40" t="s">
         <v>41</v>
@@ -2585,18 +2578,18 @@
       </c>
       <c r="G33" s="7"/>
       <c r="H33" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I33" s="51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K33" s="37"/>
     </row>
     <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="128">
+      <c r="A34" s="127">
         <v>7</v>
       </c>
-      <c r="B34" s="133"/>
+      <c r="B34" s="125"/>
       <c r="C34" s="10">
         <f>I32 + 1</f>
         <v>24</v>
@@ -2627,8 +2620,8 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="128"/>
-      <c r="B35" s="133"/>
+      <c r="A35" s="127"/>
+      <c r="B35" s="125"/>
       <c r="C35" s="10"/>
       <c r="D35" s="102" t="s">
         <v>16</v>
@@ -2644,7 +2637,7 @@
       <c r="I35" s="77"/>
     </row>
     <row r="36" spans="1:11" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="128">
+      <c r="A36" s="127">
         <v>6</v>
       </c>
       <c r="B36" s="81"/>
@@ -2679,8 +2672,8 @@
     <row r="37" spans="1:11" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="130"/>
       <c r="B37" s="82"/>
-      <c r="C37" s="116"/>
-      <c r="D37" s="115" t="s">
+      <c r="C37" s="115"/>
+      <c r="D37" s="114" t="s">
         <v>50</v>
       </c>
       <c r="E37" s="87"/>
@@ -2697,14 +2690,14 @@
       <c r="A38" s="129">
         <v>5</v>
       </c>
-      <c r="B38" s="137" t="s">
+      <c r="B38" s="122" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="48">
         <f>I36 + 1</f>
         <v>7</v>
       </c>
-      <c r="D38" s="113">
+      <c r="D38" s="112">
         <f>C38 + 1</f>
         <v>8</v>
       </c>
@@ -2730,29 +2723,29 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="128"/>
-      <c r="B39" s="138"/>
+      <c r="A39" s="127"/>
+      <c r="B39" s="123"/>
       <c r="C39" s="48"/>
       <c r="D39" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="E39" s="117" t="s">
-        <v>61</v>
+      <c r="E39" s="116" t="s">
+        <v>60</v>
       </c>
       <c r="F39" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G39" s="15"/>
-      <c r="H39" s="27" t="s">
-        <v>52</v>
+      <c r="H39" s="79" t="s">
+        <v>75</v>
       </c>
       <c r="I39" s="78"/>
     </row>
     <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="128">
+      <c r="A40" s="127">
         <v>4</v>
       </c>
-      <c r="B40" s="138"/>
+      <c r="B40" s="123"/>
       <c r="C40" s="21">
         <f>I38 + 1</f>
         <v>14</v>
@@ -2783,20 +2776,18 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="128"/>
-      <c r="B41" s="138"/>
+      <c r="A41" s="127"/>
+      <c r="B41" s="123"/>
       <c r="C41" s="47"/>
       <c r="D41" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="E41" s="106" t="s">
-        <v>62</v>
-      </c>
-      <c r="F41" s="112" t="s">
-        <v>52</v>
-      </c>
-      <c r="G41" s="57" t="s">
-        <v>6</v>
+      <c r="E41" s="15"/>
+      <c r="F41" s="105" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="106" t="s">
+        <v>61</v>
       </c>
       <c r="H41" s="54" t="s">
         <v>6</v>
@@ -2806,10 +2797,10 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="128">
+      <c r="A42" s="127">
         <v>3</v>
       </c>
-      <c r="B42" s="138"/>
+      <c r="B42" s="123"/>
       <c r="C42" s="53">
         <f>I40 + 1</f>
         <v>21</v>
@@ -2840,8 +2831,8 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="128"/>
-      <c r="B43" s="138"/>
+      <c r="A43" s="127"/>
+      <c r="B43" s="123"/>
       <c r="C43" s="53" t="s">
         <v>6</v>
       </c>
@@ -2850,7 +2841,7 @@
       </c>
       <c r="E43" s="15"/>
       <c r="F43" s="105" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="G43" s="97"/>
       <c r="H43" s="105" t="s">
@@ -2859,10 +2850,10 @@
       <c r="I43" s="94"/>
     </row>
     <row r="44" spans="1:11" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="128">
+      <c r="A44" s="127">
         <v>2</v>
       </c>
-      <c r="B44" s="138"/>
+      <c r="B44" s="123"/>
       <c r="C44" s="21">
         <f>I42 + 1</f>
         <v>28</v>
@@ -2893,12 +2884,12 @@
     </row>
     <row r="45" spans="1:11" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="130"/>
-      <c r="B45" s="138"/>
+      <c r="B45" s="123"/>
       <c r="C45" s="107"/>
       <c r="D45" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="E45" s="114"/>
+      <c r="E45" s="113"/>
       <c r="F45" s="10" t="s">
         <v>7</v>
       </c>
@@ -2913,7 +2904,7 @@
         <f>A49 + 1</f>
         <v>1</v>
       </c>
-      <c r="B46" s="132" t="s">
+      <c r="B46" s="124" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="41">
@@ -2946,8 +2937,8 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="128"/>
-      <c r="B47" s="133"/>
+      <c r="A47" s="127"/>
+      <c r="B47" s="125"/>
       <c r="C47" s="42"/>
       <c r="D47" s="7" t="s">
         <v>7</v>
@@ -2959,14 +2950,14 @@
       <c r="G47" s="49"/>
       <c r="H47" s="8"/>
       <c r="I47" s="51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="140">
+      <c r="A48" s="131">
         <v>0</v>
       </c>
-      <c r="B48" s="133"/>
+      <c r="B48" s="125"/>
       <c r="C48" s="25">
         <f>I46 + 1</f>
         <v>12</v>
@@ -2997,17 +2988,17 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="138.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="141"/>
-      <c r="B49" s="139"/>
+      <c r="A49" s="132"/>
+      <c r="B49" s="126"/>
       <c r="C49" s="12"/>
       <c r="D49" s="29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E49" s="75" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F49" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G49" s="26"/>
       <c r="H49" s="12"/>
@@ -3016,6 +3007,19 @@
     <row r="50" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B14"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B29:B35"/>
     <mergeCell ref="B38:B45"/>
     <mergeCell ref="B46:B49"/>
     <mergeCell ref="A13:A14"/>
@@ -3029,19 +3033,6 @@
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B14"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B29:B35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated schedule for mid-term peer evals
</commit_message>
<xml_diff>
--- a/CS320-Spring2019Calendar.xlsx
+++ b/CS320-Spring2019Calendar.xlsx
@@ -437,12 +437,12 @@
 AndCulture</t>
   </si>
   <si>
-    <t>CS320: SW Engineering - Spring 2019 Schedule
-(as of 4-3-2019, subject to change)</t>
-  </si>
-  <si>
     <t>Library Example Review
 (in-class)</t>
+  </si>
+  <si>
+    <t>CS320: SW Engineering - Spring 2019 Schedule
+(as of 4-8-2019, subject to change)</t>
   </si>
 </sst>
 </file>
@@ -1417,9 +1417,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1434,6 +1431,48 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1441,56 +1480,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1798,8 +1798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1812,22 +1812,22 @@
     <col min="6" max="6" width="13.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" style="4" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="13" style="3" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="133" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="135"/>
+      <c r="A1" s="121" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="123"/>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1857,10 +1857,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="129">
+      <c r="A3" s="127">
         <v>16</v>
       </c>
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="130" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="55">
@@ -1892,8 +1892,8 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="127"/>
-      <c r="B4" s="125"/>
+      <c r="A4" s="126"/>
+      <c r="B4" s="131"/>
       <c r="C4" s="53" t="s">
         <v>8</v>
       </c>
@@ -1913,10 +1913,10 @@
       <c r="I4" s="93"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="127">
+      <c r="A5" s="126">
         <v>15</v>
       </c>
-      <c r="B5" s="125"/>
+      <c r="B5" s="131"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>27</v>
@@ -1940,14 +1940,14 @@
       <c r="H5" s="91">
         <v>1</v>
       </c>
-      <c r="I5" s="117">
+      <c r="I5" s="116">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="130"/>
-      <c r="B6" s="125"/>
+      <c r="A6" s="128"/>
+      <c r="B6" s="131"/>
       <c r="C6" s="88" t="s">
         <v>54</v>
       </c>
@@ -1961,7 +1961,7 @@
       <c r="G6" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="H6" s="118" t="s">
+      <c r="H6" s="117" t="s">
         <v>44</v>
       </c>
       <c r="I6" s="51" t="s">
@@ -1969,10 +1969,10 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="129">
+      <c r="A7" s="127">
         <v>14</v>
       </c>
-      <c r="B7" s="138" t="s">
+      <c r="B7" s="132" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="91">
@@ -2005,8 +2005,8 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="128"/>
-      <c r="B8" s="139"/>
+      <c r="A8" s="129"/>
+      <c r="B8" s="133"/>
       <c r="C8" s="52" t="s">
         <v>55</v>
       </c>
@@ -2026,10 +2026,10 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="137">
+      <c r="A9" s="125">
         <v>13</v>
       </c>
-      <c r="B9" s="139"/>
+      <c r="B9" s="133"/>
       <c r="C9" s="18">
         <f>I7 + 1</f>
         <v>10</v>
@@ -2060,8 +2060,8 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="127"/>
-      <c r="B10" s="139"/>
+      <c r="A10" s="126"/>
+      <c r="B10" s="133"/>
       <c r="C10" s="52" t="s">
         <v>57</v>
       </c>
@@ -2079,10 +2079,10 @@
       <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="127">
+      <c r="A11" s="126">
         <v>12</v>
       </c>
-      <c r="B11" s="139"/>
+      <c r="B11" s="133"/>
       <c r="C11" s="21">
         <f>I9 + 1</f>
         <v>17</v>
@@ -2113,12 +2113,12 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="127"/>
-      <c r="B12" s="139"/>
+      <c r="A12" s="126"/>
+      <c r="B12" s="133"/>
       <c r="C12" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="119" t="s">
+      <c r="D12" s="118" t="s">
         <v>66</v>
       </c>
       <c r="E12" s="15"/>
@@ -2132,10 +2132,10 @@
       <c r="I12" s="94"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="127">
+      <c r="A13" s="126">
         <v>11</v>
       </c>
-      <c r="B13" s="139"/>
+      <c r="B13" s="133"/>
       <c r="C13" s="21">
         <f>I11 + 1</f>
         <v>24</v>
@@ -2159,14 +2159,14 @@
       <c r="H13" s="41">
         <v>1</v>
       </c>
-      <c r="I13" s="121">
+      <c r="I13" s="120">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="128"/>
-      <c r="B14" s="139"/>
+      <c r="A14" s="129"/>
+      <c r="B14" s="133"/>
       <c r="C14" s="96"/>
       <c r="D14" s="44" t="s">
         <v>19</v>
@@ -2184,10 +2184,10 @@
       <c r="M14" s="38"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="129">
+      <c r="A15" s="127">
         <v>10</v>
       </c>
-      <c r="B15" s="138" t="s">
+      <c r="B15" s="132" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="55">
@@ -2220,12 +2220,12 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="130"/>
-      <c r="B16" s="140"/>
+      <c r="A16" s="128"/>
+      <c r="B16" s="134"/>
       <c r="C16" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="120" t="s">
+      <c r="D16" s="119" t="s">
         <v>69</v>
       </c>
       <c r="E16" s="62" t="str">
@@ -2356,19 +2356,19 @@
       <c r="I25" s="30"/>
     </row>
     <row r="26" spans="1:11" s="32" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="133" t="str">
+      <c r="A26" s="121" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2019 Schedule
-(as of 4-3-2019, subject to change)</v>
-      </c>
-      <c r="B26" s="134"/>
-      <c r="C26" s="134"/>
-      <c r="D26" s="134"/>
-      <c r="E26" s="134"/>
-      <c r="F26" s="134"/>
-      <c r="G26" s="134"/>
-      <c r="H26" s="134"/>
-      <c r="I26" s="135"/>
+(as of 4-8-2019, subject to change)</v>
+      </c>
+      <c r="B26" s="122"/>
+      <c r="C26" s="122"/>
+      <c r="D26" s="122"/>
+      <c r="E26" s="122"/>
+      <c r="F26" s="122"/>
+      <c r="G26" s="122"/>
+      <c r="H26" s="122"/>
+      <c r="I26" s="123"/>
     </row>
     <row r="27" spans="1:11" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
@@ -2406,7 +2406,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="136">
+      <c r="A28" s="124">
         <v>10</v>
       </c>
       <c r="B28" s="80"/>
@@ -2440,8 +2440,8 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="137"/>
-      <c r="B29" s="125" t="s">
+      <c r="A29" s="125"/>
+      <c r="B29" s="131" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="101" t="s">
@@ -2473,10 +2473,10 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="137">
+      <c r="A30" s="125">
         <v>9</v>
       </c>
-      <c r="B30" s="125"/>
+      <c r="B30" s="131"/>
       <c r="C30" s="100">
         <f>I15 + 1</f>
         <v>10</v>
@@ -2507,8 +2507,8 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="127"/>
-      <c r="B31" s="125"/>
+      <c r="A31" s="126"/>
+      <c r="B31" s="131"/>
       <c r="C31" s="53" t="str">
         <f>I29</f>
         <v>WINTER BREAK</v>
@@ -2519,7 +2519,7 @@
       <c r="E31" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="F31" s="119" t="s">
+      <c r="F31" s="118" t="s">
         <v>71</v>
       </c>
       <c r="G31" s="7"/>
@@ -2532,10 +2532,10 @@
       <c r="K31" s="39"/>
     </row>
     <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="127">
+      <c r="A32" s="126">
         <v>8</v>
       </c>
-      <c r="B32" s="125"/>
+      <c r="B32" s="131"/>
       <c r="C32" s="25">
         <f>I30 + 1</f>
         <v>17</v>
@@ -2566,8 +2566,8 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="127"/>
-      <c r="B33" s="125"/>
+      <c r="A33" s="126"/>
+      <c r="B33" s="131"/>
       <c r="C33" s="10"/>
       <c r="D33" s="40" t="s">
         <v>41</v>
@@ -2586,10 +2586,10 @@
       <c r="K33" s="37"/>
     </row>
     <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="127">
+      <c r="A34" s="126">
         <v>7</v>
       </c>
-      <c r="B34" s="125"/>
+      <c r="B34" s="131"/>
       <c r="C34" s="10">
         <f>I32 + 1</f>
         <v>24</v>
@@ -2620,8 +2620,8 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="127"/>
-      <c r="B35" s="125"/>
+      <c r="A35" s="126"/>
+      <c r="B35" s="131"/>
       <c r="C35" s="10"/>
       <c r="D35" s="102" t="s">
         <v>16</v>
@@ -2637,7 +2637,7 @@
       <c r="I35" s="77"/>
     </row>
     <row r="36" spans="1:11" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="127">
+      <c r="A36" s="126">
         <v>6</v>
       </c>
       <c r="B36" s="81"/>
@@ -2670,7 +2670,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="130"/>
+      <c r="A37" s="128"/>
       <c r="B37" s="82"/>
       <c r="C37" s="115"/>
       <c r="D37" s="114" t="s">
@@ -2687,10 +2687,10 @@
       <c r="I37" s="46"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="129">
+      <c r="A38" s="127">
         <v>5</v>
       </c>
-      <c r="B38" s="122" t="s">
+      <c r="B38" s="135" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="48">
@@ -2723,29 +2723,29 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="127"/>
-      <c r="B39" s="123"/>
+      <c r="A39" s="126"/>
+      <c r="B39" s="136"/>
       <c r="C39" s="48"/>
       <c r="D39" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="E39" s="116" t="s">
-        <v>60</v>
-      </c>
+      <c r="E39" s="140"/>
       <c r="F39" s="27" t="s">
         <v>73</v>
       </c>
       <c r="G39" s="15"/>
       <c r="H39" s="79" t="s">
-        <v>75</v>
-      </c>
-      <c r="I39" s="78"/>
+        <v>74</v>
+      </c>
+      <c r="I39" s="51" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="127">
+      <c r="A40" s="126">
         <v>4</v>
       </c>
-      <c r="B40" s="123"/>
+      <c r="B40" s="136"/>
       <c r="C40" s="21">
         <f>I38 + 1</f>
         <v>14</v>
@@ -2776,8 +2776,8 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="127"/>
-      <c r="B41" s="123"/>
+      <c r="A41" s="126"/>
+      <c r="B41" s="136"/>
       <c r="C41" s="47"/>
       <c r="D41" s="108" t="s">
         <v>51</v>
@@ -2797,10 +2797,10 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="127">
+      <c r="A42" s="126">
         <v>3</v>
       </c>
-      <c r="B42" s="123"/>
+      <c r="B42" s="136"/>
       <c r="C42" s="53">
         <f>I40 + 1</f>
         <v>21</v>
@@ -2831,8 +2831,8 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="127"/>
-      <c r="B43" s="123"/>
+      <c r="A43" s="126"/>
+      <c r="B43" s="136"/>
       <c r="C43" s="53" t="s">
         <v>6</v>
       </c>
@@ -2850,10 +2850,10 @@
       <c r="I43" s="94"/>
     </row>
     <row r="44" spans="1:11" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="127">
+      <c r="A44" s="126">
         <v>2</v>
       </c>
-      <c r="B44" s="123"/>
+      <c r="B44" s="136"/>
       <c r="C44" s="21">
         <f>I42 + 1</f>
         <v>28</v>
@@ -2883,8 +2883,8 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="130"/>
-      <c r="B45" s="123"/>
+      <c r="A45" s="128"/>
+      <c r="B45" s="136"/>
       <c r="C45" s="107"/>
       <c r="D45" s="102" t="s">
         <v>40</v>
@@ -2900,11 +2900,11 @@
       <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="129">
+      <c r="A46" s="127">
         <f>A49 + 1</f>
         <v>1</v>
       </c>
-      <c r="B46" s="124" t="s">
+      <c r="B46" s="130" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="41">
@@ -2937,8 +2937,8 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="127"/>
-      <c r="B47" s="125"/>
+      <c r="A47" s="126"/>
+      <c r="B47" s="131"/>
       <c r="C47" s="42"/>
       <c r="D47" s="7" t="s">
         <v>7</v>
@@ -2954,10 +2954,10 @@
       </c>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="131">
+      <c r="A48" s="138">
         <v>0</v>
       </c>
-      <c r="B48" s="125"/>
+      <c r="B48" s="131"/>
       <c r="C48" s="25">
         <f>I46 + 1</f>
         <v>12</v>
@@ -2988,8 +2988,8 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="138.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="132"/>
-      <c r="B49" s="126"/>
+      <c r="A49" s="139"/>
+      <c r="B49" s="137"/>
       <c r="C49" s="12"/>
       <c r="D49" s="29" t="s">
         <v>53</v>
@@ -3007,6 +3007,19 @@
     <row r="50" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B38:B45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A31"/>
@@ -3020,19 +3033,6 @@
     <mergeCell ref="A26:I26"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B29:B35"/>
-    <mergeCell ref="B38:B45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>

</xml_diff>